<commit_message>
19th season - season update 7
</commit_message>
<xml_diff>
--- a/keepers 2022 (Oct  13 Edition).xlsx
+++ b/keepers 2022 (Oct  13 Edition).xlsx
@@ -21,8 +21,12 @@
     <sheet name="Sheet5" sheetId="11" state="hidden" r:id="rId12"/>
     <sheet name="Sheet6" sheetId="12" state="hidden" r:id="rId13"/>
     <sheet name="2022 leaders" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="Pivot Table_2022 leaders_1" sheetId="14" state="visible" r:id="rId15"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <pivotCaches>
+    <pivotCache cacheId="1" r:id="rId17"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -32,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2187" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2203" uniqueCount="608">
   <si>
     <t xml:space="preserve">2008/2009</t>
   </si>
@@ -1900,6 +1904,12 @@
       <t xml:space="preserve">st</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Result</t>
+  </si>
 </sst>
 </file>
 
@@ -1912,7 +1922,7 @@
     <numFmt numFmtId="167" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="168" formatCode="yyyy/mm/dd"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2117,6 +2127,11 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="15">
     <fill>
@@ -2182,7 +2197,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFBFBFBF"/>
-        <bgColor rgb="FFCCCCFF"/>
+        <bgColor rgb="FFB3B3B3"/>
       </patternFill>
     </fill>
     <fill>
@@ -2204,7 +2219,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="18">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -2269,6 +2284,76 @@
       </bottom>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="thin"/>
+      <top style="medium"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="medium"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -2313,7 +2398,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="120">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2754,6 +2839,46 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="24" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="17" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2794,7 +2919,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0070C0"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFB3B3B3"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -2819,7 +2944,7 @@
       <rgbColor rgb="FFC55A11"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FFA3A3A3"/>
-      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF004586"/>
       <rgbColor rgb="FF00B050"/>
       <rgbColor rgb="FF1B232C"/>
       <rgbColor rgb="FF212529"/>
@@ -2830,6 +2955,410 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2022 leaders'!$E$2:$E$14</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>Patrick</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Harrington</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Martin</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Symmington</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Anthony</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Duggan</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Duncan</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Egan</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Jadrian</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Kevin</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Kurtis</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Maran</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Mulvihill</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2022 leaders'!$F$2:$F$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="37816410"/>
+        <c:axId val="50874371"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="37816410"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="50874371"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50874371"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="37816410"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>28080</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>19800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>98280</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>104760</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="0" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="5826240" y="376560"/>
+        <a:ext cx="5759640" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" recordCount="13" createdVersion="3">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="E1:F14" sheet="2022 leaders"/>
+  </cacheSource>
+  <cacheFields count="2">
+    <cacheField name="GM" numFmtId="0">
+      <sharedItems count="13">
+        <s v="Anthony"/>
+        <s v="Duggan"/>
+        <s v="Duncan"/>
+        <s v="Egan"/>
+        <s v="Harrington"/>
+        <s v="Jadrian"/>
+        <s v="Kevin"/>
+        <s v="Kurtis"/>
+        <s v="Maran"/>
+        <s v="Martin"/>
+        <s v="Mulvihill"/>
+        <s v="Patrick"/>
+        <s v="Symmington"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Days in 1st" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="4" count="3">
+        <n v="0"/>
+        <n v="1"/>
+        <n v="4"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="13">
+  <r>
+    <x v="11"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="0"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DataPilot1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" useAutoFormatting="0" itemPrintTitles="1" indent="0" outline="0" outlineData="0" compact="0" compactData="0">
+  <location ref="A1:N3" firstHeaderRow="1" firstDataRow="2" firstDataCol="0"/>
+  <pivotFields count="2">
+    <pivotField axis="axisCol" compact="0" showAll="0" defaultSubtotal="0" outline="0">
+      <items count="13">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" compact="0" showAll="0" outline="0"/>
+  </pivotFields>
+  <colFields count="1">
+    <field x="0"/>
+  </colFields>
+  <dataFields count="1">
+    <dataField name="Sum - Days in 1st" fld="1" subtotal="sum" numFmtId="164"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7889,7 +8418,7 @@
   <dimension ref="A1:F200"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7922,7 +8451,7 @@
         <v>306</v>
       </c>
       <c r="F2" s="0" t="n">
-        <f aca="false">COUNTIF(B1:B400,"Patrick")</f>
+        <f aca="false">COUNTIF(B$1:B400,"Patrick")</f>
         <v>4</v>
       </c>
     </row>
@@ -7937,8 +8466,8 @@
         <v>307</v>
       </c>
       <c r="F3" s="0" t="n">
-        <f aca="false">COUNTIF(B2:B401,"Harrington")</f>
-        <v>0</v>
+        <f aca="false">COUNTIF(B$1:B401,"Harrington")</f>
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7949,10 +8478,10 @@
         <v>306</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>305</v>
+        <v>218</v>
       </c>
       <c r="F4" s="0" t="n">
-        <f aca="false">COUNTIF(B3:B402,"Symmington")</f>
+        <f aca="false">COUNTIF($B$1:B402,"Martin")</f>
         <v>1</v>
       </c>
     </row>
@@ -7964,11 +8493,11 @@
         <v>305</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>229</v>
+        <v>305</v>
       </c>
       <c r="F5" s="0" t="n">
-        <f aca="false">COUNTIF(B1:B403,"Anthony")</f>
-        <v>0</v>
+        <f aca="false">COUNTIF(B$2:B403,"Symmington")</f>
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7979,10 +8508,10 @@
         <v>306</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>304</v>
+        <v>229</v>
       </c>
       <c r="F6" s="0" t="n">
-        <f aca="false">COUNTIF(B1:B404,"Duggan")</f>
+        <f aca="false">COUNTIF(B$1:B404,"Anthony")</f>
         <v>0</v>
       </c>
     </row>
@@ -7991,11 +8520,14 @@
         <f aca="false">A6+1</f>
         <v>44848</v>
       </c>
+      <c r="B7" s="0" t="s">
+        <v>218</v>
+      </c>
       <c r="E7" s="0" t="s">
-        <v>187</v>
+        <v>304</v>
       </c>
       <c r="F7" s="0" t="n">
-        <f aca="false">COUNTIF(B1:B405,"Duncan")</f>
+        <f aca="false">COUNTIF(B$1:B405,"Duggan")</f>
         <v>0</v>
       </c>
     </row>
@@ -8005,10 +8537,10 @@
         <v>44849</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
       <c r="F8" s="0" t="n">
-        <f aca="false">COUNTIF(B4:B406,"Egan")</f>
+        <f aca="false">COUNTIF(B$1:B406,"Duncan")</f>
         <v>0</v>
       </c>
     </row>
@@ -8018,10 +8550,10 @@
         <v>44850</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>164</v>
+        <v>204</v>
       </c>
       <c r="F9" s="0" t="n">
-        <f aca="false">COUNTIF(B1:B407,"Jadrian")</f>
+        <f aca="false">COUNTIF(B$1:B407,"Egan")</f>
         <v>0</v>
       </c>
     </row>
@@ -8031,10 +8563,10 @@
         <v>44851</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>249</v>
+        <v>164</v>
       </c>
       <c r="F10" s="0" t="n">
-        <f aca="false">COUNTIF(B1:B408,"Kevin")</f>
+        <f aca="false">COUNTIF(B$1:B408,"Jadrian")</f>
         <v>0</v>
       </c>
     </row>
@@ -8044,10 +8576,10 @@
         <v>44852</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
       <c r="F11" s="0" t="n">
-        <f aca="false">COUNTIF(B1:B409,"Kurtis")</f>
+        <f aca="false">COUNTIF(B$1:B409,"Kevin")</f>
         <v>0</v>
       </c>
     </row>
@@ -8057,10 +8589,10 @@
         <v>44853</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>238</v>
+        <v>266</v>
       </c>
       <c r="F12" s="0" t="n">
-        <f aca="false">COUNTIF(B4:B410,"Maran")</f>
+        <f aca="false">COUNTIF(B$1:B410,"Kurtis")</f>
         <v>0</v>
       </c>
     </row>
@@ -8070,10 +8602,10 @@
         <v>44854</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>218</v>
+        <v>238</v>
       </c>
       <c r="F13" s="0" t="n">
-        <f aca="false">COUNTIF(B6:B411,"Martin")</f>
+        <f aca="false">COUNTIF(B$1:B411,"Maran")</f>
         <v>0</v>
       </c>
     </row>
@@ -8086,7 +8618,7 @@
         <v>118</v>
       </c>
       <c r="F14" s="0" t="n">
-        <f aca="false">COUNTIF(B9:B412,"Mulvihill")</f>
+        <f aca="false">COUNTIF(B$1:B412,"Mulvihill")</f>
         <v>0</v>
       </c>
     </row>
@@ -9204,6 +9736,137 @@
       <c r="A200" s="108" t="n">
         <f aca="false">A199+1</f>
         <v>45041</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:N3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="110" t="s">
+        <v>606</v>
+      </c>
+      <c r="B1" s="111"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
+      <c r="F1" s="111"/>
+      <c r="G1" s="111"/>
+      <c r="H1" s="111"/>
+      <c r="I1" s="111"/>
+      <c r="J1" s="111"/>
+      <c r="K1" s="111"/>
+      <c r="L1" s="111"/>
+      <c r="M1" s="111"/>
+      <c r="N1" s="112"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="113" t="s">
+        <v>229</v>
+      </c>
+      <c r="B2" s="114" t="s">
+        <v>304</v>
+      </c>
+      <c r="C2" s="114" t="s">
+        <v>187</v>
+      </c>
+      <c r="D2" s="114" t="s">
+        <v>204</v>
+      </c>
+      <c r="E2" s="114" t="s">
+        <v>307</v>
+      </c>
+      <c r="F2" s="114" t="s">
+        <v>164</v>
+      </c>
+      <c r="G2" s="114" t="s">
+        <v>249</v>
+      </c>
+      <c r="H2" s="114" t="s">
+        <v>266</v>
+      </c>
+      <c r="I2" s="114" t="s">
+        <v>238</v>
+      </c>
+      <c r="J2" s="114" t="s">
+        <v>218</v>
+      </c>
+      <c r="K2" s="114" t="s">
+        <v>118</v>
+      </c>
+      <c r="L2" s="114" t="s">
+        <v>306</v>
+      </c>
+      <c r="M2" s="114" t="s">
+        <v>305</v>
+      </c>
+      <c r="N2" s="115" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="116" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" s="117" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="117" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="117" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="117" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="117" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="117" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="117" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="117" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="117" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="117" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="117" t="n">
+        <v>4</v>
+      </c>
+      <c r="M3" s="118" t="n">
+        <v>1</v>
+      </c>
+      <c r="N3" s="119" t="n">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -14555,7 +15218,7 @@
       </c>
       <c r="B1" s="0" t="n">
         <f aca="true">RAND()*100</f>
-        <v>92.5602012062413</v>
+        <v>45.2069368161492</v>
       </c>
       <c r="AA1" s="0" t="s">
         <v>307</v>
@@ -14603,7 +15266,7 @@
       </c>
       <c r="B2" s="0" t="n">
         <f aca="true">RAND()*100</f>
-        <v>70.5897535724673</v>
+        <v>27.2143069893543</v>
       </c>
       <c r="AB2" s="0" t="s">
         <v>164</v>
@@ -14648,7 +15311,7 @@
       </c>
       <c r="B3" s="0" t="n">
         <f aca="true">RAND()*100</f>
-        <v>68.8594108963583</v>
+        <v>75.1651137209133</v>
       </c>
       <c r="AC3" s="0" t="s">
         <v>306</v>

</xml_diff>

<commit_message>
19th season - season update 8
</commit_message>
<xml_diff>
--- a/keepers 2022 (Oct  13 Edition).xlsx
+++ b/keepers 2022 (Oct  13 Edition).xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2203" uniqueCount="608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2206" uniqueCount="608">
   <si>
     <t xml:space="preserve">2008/2009</t>
   </si>
@@ -2957,7 +2957,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3009,37 +3009,37 @@
                   <c:v>Patrick</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Harrington</c:v>
+                  <c:v>Maran</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Martin</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>Harrington</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>Symmington</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Anthony</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Duggan</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Duncan</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>Egan</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>Jadrian</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>Kevin</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>Kurtis</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Maran</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>Mulvihill</c:v>
@@ -3057,16 +3057,16 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -3098,11 +3098,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="37816410"/>
-        <c:axId val="50874371"/>
+        <c:axId val="75824534"/>
+        <c:axId val="18878471"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="37816410"/>
+        <c:axId val="75824534"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3130,7 +3130,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50874371"/>
+        <c:crossAx val="18878471"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3138,7 +3138,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50874371"/>
+        <c:axId val="18878471"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3175,7 +3175,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37816410"/>
+        <c:crossAx val="75824534"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3368,10 +3368,10 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="L20" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+      <selection pane="topRight" activeCell="U39" activeCellId="0" sqref="U39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.55859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8418,7 +8418,7 @@
   <dimension ref="A1:F200"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+      <selection pane="topLeft" activeCell="H23" activeCellId="0" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8463,11 +8463,11 @@
         <v>306</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>307</v>
+        <v>238</v>
       </c>
       <c r="F3" s="0" t="n">
-        <f aca="false">COUNTIF(B$1:B401,"Harrington")</f>
-        <v>1</v>
+        <f aca="false">COUNTIF(B$1:B401,"Maran")</f>
+        <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8482,7 +8482,7 @@
       </c>
       <c r="F4" s="0" t="n">
         <f aca="false">COUNTIF($B$1:B402,"Martin")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8493,10 +8493,10 @@
         <v>305</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="F5" s="0" t="n">
-        <f aca="false">COUNTIF(B$2:B403,"Symmington")</f>
+        <f aca="false">COUNTIF(B$1:B403,"Harrington")</f>
         <v>1</v>
       </c>
     </row>
@@ -8508,11 +8508,11 @@
         <v>306</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>229</v>
+        <v>305</v>
       </c>
       <c r="F6" s="0" t="n">
-        <f aca="false">COUNTIF(B$1:B404,"Anthony")</f>
-        <v>0</v>
+        <f aca="false">COUNTIF(B$2:B404,"Symmington")</f>
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8524,10 +8524,10 @@
         <v>218</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>304</v>
+        <v>229</v>
       </c>
       <c r="F7" s="0" t="n">
-        <f aca="false">COUNTIF(B$1:B405,"Duggan")</f>
+        <f aca="false">COUNTIF(B$1:B405,"Anthony")</f>
         <v>0</v>
       </c>
     </row>
@@ -8536,11 +8536,14 @@
         <f aca="false">A7+1</f>
         <v>44849</v>
       </c>
+      <c r="B8" s="0" t="s">
+        <v>218</v>
+      </c>
       <c r="E8" s="0" t="s">
-        <v>187</v>
+        <v>304</v>
       </c>
       <c r="F8" s="0" t="n">
-        <f aca="false">COUNTIF(B$1:B406,"Duncan")</f>
+        <f aca="false">COUNTIF(B$1:B406,"Duggan")</f>
         <v>0</v>
       </c>
     </row>
@@ -8549,11 +8552,14 @@
         <f aca="false">A8+1</f>
         <v>44850</v>
       </c>
+      <c r="B9" s="0" t="s">
+        <v>238</v>
+      </c>
       <c r="E9" s="0" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
       <c r="F9" s="0" t="n">
-        <f aca="false">COUNTIF(B$1:B407,"Egan")</f>
+        <f aca="false">COUNTIF(B$1:B407,"Duncan")</f>
         <v>0</v>
       </c>
     </row>
@@ -8562,11 +8568,14 @@
         <f aca="false">A9+1</f>
         <v>44851</v>
       </c>
+      <c r="B10" s="0" t="s">
+        <v>238</v>
+      </c>
       <c r="E10" s="0" t="s">
-        <v>164</v>
+        <v>204</v>
       </c>
       <c r="F10" s="0" t="n">
-        <f aca="false">COUNTIF(B$1:B408,"Jadrian")</f>
+        <f aca="false">COUNTIF(B$1:B408,"Egan")</f>
         <v>0</v>
       </c>
     </row>
@@ -8576,10 +8585,10 @@
         <v>44852</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>249</v>
+        <v>164</v>
       </c>
       <c r="F11" s="0" t="n">
-        <f aca="false">COUNTIF(B$1:B409,"Kevin")</f>
+        <f aca="false">COUNTIF(B$1:B409,"Jadrian")</f>
         <v>0</v>
       </c>
     </row>
@@ -8589,10 +8598,10 @@
         <v>44853</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
       <c r="F12" s="0" t="n">
-        <f aca="false">COUNTIF(B$1:B410,"Kurtis")</f>
+        <f aca="false">COUNTIF(B$1:B410,"Kevin")</f>
         <v>0</v>
       </c>
     </row>
@@ -8602,10 +8611,10 @@
         <v>44854</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>238</v>
+        <v>266</v>
       </c>
       <c r="F13" s="0" t="n">
-        <f aca="false">COUNTIF(B$1:B411,"Maran")</f>
+        <f aca="false">COUNTIF(B$1:B411,"Kurtis")</f>
         <v>0</v>
       </c>
     </row>
@@ -15218,7 +15227,7 @@
       </c>
       <c r="B1" s="0" t="n">
         <f aca="true">RAND()*100</f>
-        <v>45.2069368161492</v>
+        <v>87.2716796517392</v>
       </c>
       <c r="AA1" s="0" t="s">
         <v>307</v>
@@ -15266,7 +15275,7 @@
       </c>
       <c r="B2" s="0" t="n">
         <f aca="true">RAND()*100</f>
-        <v>27.2143069893543</v>
+        <v>98.0642092699216</v>
       </c>
       <c r="AB2" s="0" t="s">
         <v>164</v>
@@ -15311,7 +15320,7 @@
       </c>
       <c r="B3" s="0" t="n">
         <f aca="true">RAND()*100</f>
-        <v>75.1651137209133</v>
+        <v>87.9279519258254</v>
       </c>
       <c r="AC3" s="0" t="s">
         <v>306</v>

</xml_diff>

<commit_message>
19th season - season update 9
</commit_message>
<xml_diff>
--- a/keepers 2022 (Oct  13 Edition).xlsx
+++ b/keepers 2022 (Oct  13 Edition).xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2206" uniqueCount="608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2208" uniqueCount="608">
   <si>
     <t xml:space="preserve">2008/2009</t>
   </si>
@@ -2957,7 +2957,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3054,10 +3054,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2</c:v>
@@ -3098,11 +3098,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="75824534"/>
-        <c:axId val="18878471"/>
+        <c:axId val="55882937"/>
+        <c:axId val="38340801"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="75824534"/>
+        <c:axId val="55882937"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3130,7 +3130,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="18878471"/>
+        <c:crossAx val="38340801"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3138,7 +3138,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="18878471"/>
+        <c:axId val="38340801"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3175,7 +3175,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75824534"/>
+        <c:crossAx val="55882937"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8418,7 +8418,7 @@
   <dimension ref="A1:F200"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H23" activeCellId="0" sqref="H23"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8452,7 +8452,7 @@
       </c>
       <c r="F2" s="0" t="n">
         <f aca="false">COUNTIF(B$1:B400,"Patrick")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8467,7 +8467,7 @@
       </c>
       <c r="F3" s="0" t="n">
         <f aca="false">COUNTIF(B$1:B401,"Maran")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8584,6 +8584,9 @@
         <f aca="false">A10+1</f>
         <v>44852</v>
       </c>
+      <c r="B11" s="0" t="s">
+        <v>306</v>
+      </c>
       <c r="E11" s="0" t="s">
         <v>164</v>
       </c>
@@ -8596,6 +8599,9 @@
       <c r="A12" s="108" t="n">
         <f aca="false">A11+1</f>
         <v>44853</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>238</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>249</v>
@@ -15227,7 +15233,7 @@
       </c>
       <c r="B1" s="0" t="n">
         <f aca="true">RAND()*100</f>
-        <v>87.2716796517392</v>
+        <v>66.4615254497833</v>
       </c>
       <c r="AA1" s="0" t="s">
         <v>307</v>
@@ -15275,7 +15281,7 @@
       </c>
       <c r="B2" s="0" t="n">
         <f aca="true">RAND()*100</f>
-        <v>98.0642092699216</v>
+        <v>7.39097218238778</v>
       </c>
       <c r="AB2" s="0" t="s">
         <v>164</v>
@@ -15320,7 +15326,7 @@
       </c>
       <c r="B3" s="0" t="n">
         <f aca="true">RAND()*100</f>
-        <v>87.9279519258254</v>
+        <v>27.925930880808</v>
       </c>
       <c r="AC3" s="0" t="s">
         <v>306</v>

</xml_diff>

<commit_message>
19th season - season update 10
</commit_message>
<xml_diff>
--- a/keepers 2022 (Oct  13 Edition).xlsx
+++ b/keepers 2022 (Oct  13 Edition).xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2208" uniqueCount="608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2210" uniqueCount="608">
   <si>
     <t xml:space="preserve">2008/2009</t>
   </si>
@@ -2957,7 +2957,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3057,7 +3057,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2</c:v>
@@ -3098,11 +3098,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="55882937"/>
-        <c:axId val="38340801"/>
+        <c:axId val="52046688"/>
+        <c:axId val="81777703"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="55882937"/>
+        <c:axId val="52046688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3130,7 +3130,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38340801"/>
+        <c:crossAx val="81777703"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3138,7 +3138,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="38340801"/>
+        <c:axId val="81777703"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3175,7 +3175,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55882937"/>
+        <c:crossAx val="52046688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8418,7 +8418,7 @@
   <dimension ref="A1:F200"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8467,7 +8467,7 @@
       </c>
       <c r="F3" s="0" t="n">
         <f aca="false">COUNTIF(B$1:B401,"Maran")</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8616,6 +8616,9 @@
         <f aca="false">A12+1</f>
         <v>44854</v>
       </c>
+      <c r="B13" s="0" t="s">
+        <v>238</v>
+      </c>
       <c r="E13" s="0" t="s">
         <v>266</v>
       </c>
@@ -8628,6 +8631,9 @@
       <c r="A14" s="108" t="n">
         <f aca="false">A13+1</f>
         <v>44855</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>238</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>118</v>
@@ -15233,7 +15239,7 @@
       </c>
       <c r="B1" s="0" t="n">
         <f aca="true">RAND()*100</f>
-        <v>66.4615254497833</v>
+        <v>75.3307964170831</v>
       </c>
       <c r="AA1" s="0" t="s">
         <v>307</v>
@@ -15281,7 +15287,7 @@
       </c>
       <c r="B2" s="0" t="n">
         <f aca="true">RAND()*100</f>
-        <v>7.39097218238778</v>
+        <v>44.114142116158</v>
       </c>
       <c r="AB2" s="0" t="s">
         <v>164</v>
@@ -15326,7 +15332,7 @@
       </c>
       <c r="B3" s="0" t="n">
         <f aca="true">RAND()*100</f>
-        <v>27.925930880808</v>
+        <v>60.1848928206436</v>
       </c>
       <c r="AC3" s="0" t="s">
         <v>306</v>

</xml_diff>

<commit_message>
20th season - 14th summer update
</commit_message>
<xml_diff>
--- a/keepers 2022 (Oct  13 Edition).xlsx
+++ b/keepers 2022 (Oct  13 Edition).xlsx
@@ -1010,6 +1010,7 @@
         <color rgb="FF0070C0"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(Names in </t>
     </r>
@@ -1019,6 +1020,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">red</t>
     </r>
@@ -1028,6 +1030,7 @@
         <color rgb="FF0070C0"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> were kept last year and only have 1 eligible year remaining )</t>
     </r>
@@ -1918,6 +1921,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Days in 1</t>
     </r>
@@ -1928,6 +1932,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">st</t>
     </r>
@@ -2024,6 +2029,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2046,18 +2052,21 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -2065,12 +2074,14 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -2078,6 +2089,7 @@
       <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -2085,29 +2097,34 @@
       <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFFFF00"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -2115,6 +2132,7 @@
       <color rgb="FF212529"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -2123,6 +2141,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <strike val="true"/>
@@ -2130,6 +2149,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <strike val="true"/>
@@ -2137,6 +2157,7 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -2145,12 +2166,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -2158,6 +2181,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -2166,6 +2190,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <strike val="true"/>
@@ -2173,23 +2198,27 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <vertAlign val="superscript"/>
@@ -2197,6 +2226,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -3176,11 +3206,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="58940979"/>
-        <c:axId val="46335098"/>
+        <c:axId val="11536922"/>
+        <c:axId val="46911082"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="58940979"/>
+        <c:axId val="11536922"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3208,7 +3238,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46335098"/>
+        <c:crossAx val="46911082"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3216,7 +3246,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46335098"/>
+        <c:axId val="46911082"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3253,7 +3283,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58940979"/>
+        <c:crossAx val="11536922"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3291,9 +3321,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>101520</xdr:colOff>
+      <xdr:colOff>101160</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>93960</xdr:rowOff>
+      <xdr:rowOff>93600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3301,8 +3331,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5836320" y="376560"/>
-        <a:ext cx="5761080" cy="3236400"/>
+        <a:off x="5840280" y="376560"/>
+        <a:ext cx="5765040" cy="3236040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3452,10 +3482,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="R6" activeCellId="0" sqref="R6"/>
+      <selection pane="topRight" activeCell="R1" activeCellId="0" sqref="R1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15"/>
@@ -4938,7 +4968,7 @@
       <c r="Q38" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="R38" s="7" t="s">
+      <c r="R38" s="3" t="s">
         <v>193</v>
       </c>
     </row>
@@ -6074,7 +6104,7 @@
       <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="8.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.44"/>
@@ -7270,7 +7300,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.55"/>
@@ -7971,7 +8001,7 @@
       <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.66"/>
@@ -8605,7 +8635,7 @@
       <selection pane="topLeft" activeCell="T155" activeCellId="0" sqref="T155"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.36"/>
   </cols>
@@ -10521,7 +10551,7 @@
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="110" t="s">
@@ -10651,7 +10681,7 @@
       <selection pane="topLeft" activeCell="E33" activeCellId="0" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.21"/>
@@ -13328,7 +13358,7 @@
       <selection pane="topLeft" activeCell="K31" activeCellId="0" sqref="K31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="8.54"/>
   </cols>
@@ -15600,7 +15630,7 @@
       <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="8.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.44"/>
@@ -15777,7 +15807,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="8.54"/>
   </cols>
@@ -15974,7 +16004,7 @@
       <selection pane="topLeft" activeCell="AD14" activeCellId="0" sqref="AD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="0" width="8.54"/>
@@ -15992,7 +16022,7 @@
       </c>
       <c r="B1" s="0" t="n">
         <f aca="true">RAND()*100</f>
-        <v>14.7027385380138</v>
+        <v>74.4590456841612</v>
       </c>
       <c r="AA1" s="0" t="s">
         <v>318</v>
@@ -16040,7 +16070,7 @@
       </c>
       <c r="B2" s="0" t="n">
         <f aca="true">RAND()*100</f>
-        <v>40.26155787237</v>
+        <v>50.3607051855345</v>
       </c>
       <c r="AB2" s="0" t="s">
         <v>169</v>
@@ -16085,7 +16115,7 @@
       </c>
       <c r="B3" s="0" t="n">
         <f aca="true">RAND()*100</f>
-        <v>97.0843827861539</v>
+        <v>27.162771392206</v>
       </c>
       <c r="AC3" s="0" t="s">
         <v>317</v>
@@ -16383,7 +16413,7 @@
       <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.33"/>
@@ -19418,7 +19448,7 @@
       <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="1" style="0" width="8.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.44"/>

</xml_diff>

<commit_message>
21st season - New Website 14
</commit_message>
<xml_diff>
--- a/keepers 2022 (Oct  13 Edition).xlsx
+++ b/keepers 2022 (Oct  13 Edition).xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="1" state="visible" r:id="rId2"/>
@@ -2173,6 +2173,9 @@
     <t xml:space="preserve">Last</t>
   </si>
   <si>
+    <t xml:space="preserve">10(last)</t>
+  </si>
+  <si>
     <t xml:space="preserve">12(last)</t>
   </si>
   <si>
@@ -2180,9 +2183,6 @@
   </si>
   <si>
     <t xml:space="preserve">14(last)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10(last)</t>
   </si>
   <si>
     <t xml:space="preserve">11(last)</t>
@@ -3220,15 +3220,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="30" fillId="18" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3310,7 +3310,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3452,11 +3452,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="35611832"/>
-        <c:axId val="31566457"/>
+        <c:axId val="89843127"/>
+        <c:axId val="47963996"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="35611832"/>
+        <c:axId val="89843127"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3484,7 +3484,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31566457"/>
+        <c:crossAx val="47963996"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3492,7 +3492,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="31566457"/>
+        <c:axId val="47963996"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3529,7 +3529,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35611832"/>
+        <c:crossAx val="89843127"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3725,7 +3725,7 @@
   </sheetPr>
   <dimension ref="A1:T96"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
@@ -6768,7 +6768,7 @@
   </sheetPr>
   <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
@@ -7964,7 +7964,7 @@
   </sheetPr>
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -8665,7 +8665,7 @@
   </sheetPr>
   <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -9299,7 +9299,7 @@
   </sheetPr>
   <dimension ref="A1:L200"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A130" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A130" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="T155" activeCellId="0" sqref="T155"/>
     </sheetView>
   </sheetViews>
@@ -11215,7 +11215,7 @@
   </sheetPr>
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -11345,8 +11345,8 @@
   </sheetPr>
   <dimension ref="A1:AA59"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12304,11 +12304,6 @@
       <c r="O22" s="125"/>
       <c r="P22" s="125"/>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AA26" s="124" t="n">
-        <v>2024</v>
-      </c>
-    </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="124" t="s">
         <v>689</v>
@@ -12388,90 +12383,93 @@
       <c r="Z32" s="124" t="n">
         <v>2023</v>
       </c>
+      <c r="AA32" s="124" t="n">
+        <v>2024</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="124" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B33" s="125" t="n">
-        <f aca="false">COUNTIF(G27:BA27,"&lt;&gt;")</f>
-        <v>0</v>
+        <f aca="false">COUNTIF(G33:BA33,"&lt;&gt;")</f>
+        <v>20</v>
       </c>
       <c r="C33" s="125" t="n">
-        <f aca="false">COUNTIF(G27:BB27,"1")</f>
-        <v>0</v>
+        <f aca="false">COUNTIF(G33:BB33,"1")</f>
+        <v>2</v>
       </c>
       <c r="D33" s="125" t="n">
-        <f aca="false">COUNTIF(G27:BC27,"2")</f>
-        <v>0</v>
+        <f aca="false">COUNTIF(G33:BC33,"2")</f>
+        <v>2</v>
       </c>
       <c r="E33" s="125" t="n">
-        <f aca="false">COUNTIF(G27:BD27,"3")</f>
-        <v>0</v>
+        <f aca="false">COUNTIF(G33:BD33,"3")</f>
+        <v>4</v>
       </c>
       <c r="F33" s="125" t="n">
-        <f aca="false">COUNTIF(G27:BC27,"*last*")</f>
-        <v>0</v>
+        <f aca="false">COUNTIF(G33:BC33,"*last*")</f>
+        <v>1</v>
       </c>
       <c r="G33" s="125" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="H33" s="125" t="n">
+        <v>10</v>
+      </c>
+      <c r="I33" s="125" t="s">
+        <v>695</v>
+      </c>
+      <c r="J33" s="125" t="n">
+        <v>7</v>
+      </c>
+      <c r="K33" s="125" t="n">
+        <v>7</v>
+      </c>
+      <c r="L33" s="125" t="n">
+        <v>5</v>
+      </c>
+      <c r="M33" s="125" t="n">
+        <v>5</v>
+      </c>
+      <c r="N33" s="125" t="n">
+        <v>1</v>
+      </c>
+      <c r="O33" s="125" t="n">
         <v>11</v>
       </c>
-      <c r="I33" s="125" t="n">
-        <v>7</v>
-      </c>
-      <c r="J33" s="125" t="n">
-        <v>6</v>
-      </c>
-      <c r="K33" s="125" t="n">
+      <c r="P33" s="125" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q33" s="125" t="n">
+        <v>2</v>
+      </c>
+      <c r="R33" s="125" t="n">
+        <v>5</v>
+      </c>
+      <c r="S33" s="125" t="n">
+        <v>3</v>
+      </c>
+      <c r="T33" s="125" t="n">
+        <v>2</v>
+      </c>
+      <c r="U33" s="125" t="n">
+        <v>3</v>
+      </c>
+      <c r="V33" s="125" t="n">
+        <v>3</v>
+      </c>
+      <c r="W33" s="125" t="n">
         <v>9</v>
       </c>
-      <c r="L33" s="125" t="n">
-        <v>2</v>
-      </c>
-      <c r="M33" s="125" t="n">
+      <c r="X33" s="125" t="n">
         <v>4</v>
       </c>
-      <c r="N33" s="125" t="n">
-        <v>5</v>
-      </c>
-      <c r="O33" s="125" t="n">
-        <v>1</v>
-      </c>
-      <c r="P33" s="125" t="n">
-        <v>8</v>
-      </c>
-      <c r="Q33" s="125" t="n">
-        <v>3</v>
-      </c>
-      <c r="R33" s="125" t="n">
-        <v>2</v>
-      </c>
-      <c r="S33" s="125" t="n">
-        <v>2</v>
-      </c>
-      <c r="T33" s="125" t="n">
-        <v>4</v>
-      </c>
-      <c r="U33" s="125" t="n">
-        <v>6</v>
-      </c>
-      <c r="V33" s="125" t="n">
-        <v>8</v>
-      </c>
-      <c r="W33" s="125" t="n">
-        <v>5</v>
-      </c>
-      <c r="X33" s="125" t="n">
-        <v>11</v>
-      </c>
       <c r="Y33" s="125" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Z33" s="125" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12479,23 +12477,23 @@
         <v>356</v>
       </c>
       <c r="B34" s="125" t="n">
-        <f aca="false">COUNTIF(G28:BA28,"&lt;&gt;")</f>
-        <v>0</v>
+        <f aca="false">COUNTIF(G34:BA34,"&lt;&gt;")</f>
+        <v>20</v>
       </c>
       <c r="C34" s="125" t="n">
-        <f aca="false">COUNTIF(G28:BB28,"1")</f>
-        <v>0</v>
+        <f aca="false">COUNTIF(G34:BB34,"1")</f>
+        <v>9</v>
       </c>
       <c r="D34" s="125" t="n">
-        <f aca="false">COUNTIF(G28:BC28,"2")</f>
-        <v>0</v>
+        <f aca="false">COUNTIF(G34:BC34,"2")</f>
+        <v>5</v>
       </c>
       <c r="E34" s="125" t="n">
-        <f aca="false">COUNTIF(G28:BD28,"3")</f>
-        <v>0</v>
+        <f aca="false">COUNTIF(G34:BD34,"3")</f>
+        <v>3</v>
       </c>
       <c r="F34" s="125" t="n">
-        <f aca="false">COUNTIF(G28:BC28,"*last*")</f>
+        <f aca="false">COUNTIF(G34:BC34,"*last*")</f>
         <v>0</v>
       </c>
       <c r="G34" s="125" t="n">
@@ -12564,30 +12562,30 @@
         <v>119</v>
       </c>
       <c r="B35" s="125" t="n">
-        <f aca="false">COUNTIF(G29:BA29,"&lt;&gt;")</f>
+        <f aca="false">COUNTIF(G35:BA35,"&lt;&gt;")</f>
+        <v>20</v>
+      </c>
+      <c r="C35" s="125" t="n">
+        <f aca="false">COUNTIF(G35:BB35,"1")</f>
+        <v>1</v>
+      </c>
+      <c r="D35" s="125" t="n">
+        <f aca="false">COUNTIF(G35:BC35,"2")</f>
         <v>0</v>
       </c>
-      <c r="C35" s="125" t="n">
-        <f aca="false">COUNTIF(G29:BB29,"1")</f>
-        <v>0</v>
-      </c>
-      <c r="D35" s="125" t="n">
-        <f aca="false">COUNTIF(G29:BC29,"2")</f>
-        <v>0</v>
-      </c>
       <c r="E35" s="125" t="n">
-        <f aca="false">COUNTIF(G29:BD29,"3")</f>
-        <v>0</v>
+        <f aca="false">COUNTIF(G35:BD35,"3")</f>
+        <v>2</v>
       </c>
       <c r="F35" s="125" t="n">
-        <f aca="false">COUNTIF(G29:BC29,"*last*")</f>
-        <v>0</v>
+        <f aca="false">COUNTIF(G35:BC35,"*last*")</f>
+        <v>3</v>
       </c>
       <c r="G35" s="125" t="n">
         <v>5</v>
       </c>
       <c r="H35" s="125" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="I35" s="125" t="n">
         <v>5</v>
@@ -12608,7 +12606,7 @@
         <v>8</v>
       </c>
       <c r="O35" s="125" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="P35" s="125" t="n">
         <v>9</v>
@@ -12617,7 +12615,7 @@
         <v>6</v>
       </c>
       <c r="R35" s="125" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="S35" s="125" t="n">
         <v>13</v>
@@ -12646,356 +12644,356 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="124" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B36" s="125" t="n">
-        <f aca="false">COUNTIF(G30:BA30,"&lt;&gt;")</f>
+        <f aca="false">COUNTIF(G36:BA36,"&lt;&gt;")</f>
+        <v>20</v>
+      </c>
+      <c r="C36" s="125" t="n">
+        <f aca="false">COUNTIF(G36:BB36,"1")</f>
+        <v>2</v>
+      </c>
+      <c r="D36" s="125" t="n">
+        <f aca="false">COUNTIF(G36:BC36,"2")</f>
+        <v>3</v>
+      </c>
+      <c r="E36" s="125" t="n">
+        <f aca="false">COUNTIF(G36:BD36,"3")</f>
+        <v>1</v>
+      </c>
+      <c r="F36" s="125" t="n">
+        <f aca="false">COUNTIF(G36:BC36,"*last*")</f>
         <v>0</v>
       </c>
-      <c r="C36" s="125" t="n">
-        <f aca="false">COUNTIF(G30:BB30,"1")</f>
-        <v>0</v>
-      </c>
-      <c r="D36" s="125" t="n">
-        <f aca="false">COUNTIF(G30:BC30,"2")</f>
-        <v>0</v>
-      </c>
-      <c r="E36" s="125" t="n">
-        <f aca="false">COUNTIF(G30:BD30,"3")</f>
-        <v>0</v>
-      </c>
-      <c r="F36" s="125" t="n">
-        <f aca="false">COUNTIF(G30:BC30,"*last*")</f>
-        <v>0</v>
-      </c>
       <c r="G36" s="125" t="n">
+        <v>1</v>
+      </c>
+      <c r="H36" s="125" t="n">
+        <v>11</v>
+      </c>
+      <c r="I36" s="125" t="n">
+        <v>7</v>
+      </c>
+      <c r="J36" s="125" t="n">
+        <v>6</v>
+      </c>
+      <c r="K36" s="125" t="n">
         <v>9</v>
       </c>
-      <c r="H36" s="125" t="n">
-        <v>10</v>
-      </c>
-      <c r="I36" s="125" t="s">
-        <v>698</v>
-      </c>
-      <c r="J36" s="125" t="n">
-        <v>7</v>
-      </c>
-      <c r="K36" s="125" t="n">
-        <v>7</v>
-      </c>
       <c r="L36" s="125" t="n">
+        <v>2</v>
+      </c>
+      <c r="M36" s="125" t="n">
+        <v>4</v>
+      </c>
+      <c r="N36" s="125" t="n">
         <v>5</v>
       </c>
-      <c r="M36" s="125" t="n">
+      <c r="O36" s="125" t="n">
+        <v>1</v>
+      </c>
+      <c r="P36" s="125" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q36" s="125" t="n">
+        <v>3</v>
+      </c>
+      <c r="R36" s="125" t="n">
+        <v>2</v>
+      </c>
+      <c r="S36" s="125" t="n">
+        <v>2</v>
+      </c>
+      <c r="T36" s="125" t="n">
+        <v>4</v>
+      </c>
+      <c r="U36" s="125" t="n">
+        <v>6</v>
+      </c>
+      <c r="V36" s="125" t="n">
+        <v>8</v>
+      </c>
+      <c r="W36" s="125" t="n">
         <v>5</v>
       </c>
-      <c r="N36" s="125" t="n">
-        <v>1</v>
-      </c>
-      <c r="O36" s="125" t="n">
+      <c r="X36" s="125" t="n">
         <v>11</v>
       </c>
-      <c r="P36" s="125" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q36" s="125" t="n">
-        <v>2</v>
-      </c>
-      <c r="R36" s="125" t="n">
-        <v>5</v>
-      </c>
-      <c r="S36" s="125" t="n">
-        <v>3</v>
-      </c>
-      <c r="T36" s="125" t="n">
-        <v>2</v>
-      </c>
-      <c r="U36" s="125" t="n">
-        <v>3</v>
-      </c>
-      <c r="V36" s="125" t="n">
-        <v>3</v>
-      </c>
-      <c r="W36" s="125" t="n">
-        <v>9</v>
-      </c>
-      <c r="X36" s="125" t="n">
-        <v>4</v>
-      </c>
       <c r="Y36" s="125" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Z36" s="125" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="124" t="s">
-        <v>313</v>
+        <v>355</v>
       </c>
       <c r="B37" s="125" t="n">
-        <f aca="false">COUNTIF(G31:BA31,"&lt;&gt;")</f>
-        <v>0</v>
+        <f aca="false">COUNTIF(G37:BA37,"&lt;&gt;")</f>
+        <v>19</v>
       </c>
       <c r="C37" s="125" t="n">
-        <f aca="false">COUNTIF(G31:BB31,"1")</f>
-        <v>0</v>
+        <f aca="false">COUNTIF(G37:BB37,"1")</f>
+        <v>2</v>
       </c>
       <c r="D37" s="125" t="n">
-        <f aca="false">COUNTIF(G31:BC31,"2")</f>
-        <v>0</v>
+        <f aca="false">COUNTIF(G37:BC37,"2")</f>
+        <v>1</v>
       </c>
       <c r="E37" s="125" t="n">
-        <f aca="false">COUNTIF(G31:BD31,"3")</f>
-        <v>0</v>
+        <f aca="false">COUNTIF(G37:BD37,"3")</f>
+        <v>2</v>
       </c>
       <c r="F37" s="125" t="n">
-        <f aca="false">COUNTIF(G31:BC31,"*last*")</f>
-        <v>0</v>
+        <f aca="false">COUNTIF(G37:BC37,"*last*")</f>
+        <v>1</v>
       </c>
       <c r="G37" s="125" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="H37" s="125" t="n">
+        <v>3</v>
+      </c>
+      <c r="I37" s="126"/>
+      <c r="J37" s="127" t="n">
+        <v>11</v>
+      </c>
+      <c r="K37" s="125" t="n">
+        <v>6</v>
+      </c>
+      <c r="L37" s="125" t="n">
+        <v>7</v>
+      </c>
+      <c r="M37" s="125" t="n">
+        <v>2</v>
+      </c>
+      <c r="N37" s="125" t="n">
+        <v>3</v>
+      </c>
+      <c r="O37" s="125" t="n">
+        <v>5</v>
+      </c>
+      <c r="P37" s="125" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q37" s="125" t="n">
         <v>8</v>
       </c>
-      <c r="I37" s="125" t="n">
-        <v>8</v>
-      </c>
-      <c r="J37" s="125" t="n">
+      <c r="R37" s="125" t="n">
+        <v>1</v>
+      </c>
+      <c r="S37" s="125" t="n">
+        <v>11</v>
+      </c>
+      <c r="T37" s="125" t="n">
+        <v>1</v>
+      </c>
+      <c r="U37" s="125" t="n">
+        <v>12</v>
+      </c>
+      <c r="V37" s="125" t="n">
+        <v>7</v>
+      </c>
+      <c r="W37" s="125" t="n">
         <v>4</v>
       </c>
-      <c r="K37" s="125" t="n">
-        <v>10</v>
-      </c>
-      <c r="L37" s="125" t="n">
-        <v>10</v>
-      </c>
-      <c r="M37" s="125" t="n">
+      <c r="X37" s="125" t="n">
+        <v>5</v>
+      </c>
+      <c r="Y37" s="125" t="s">
+        <v>697</v>
+      </c>
+      <c r="Z37" s="125" t="n">
         <v>9</v>
       </c>
-      <c r="N37" s="125" t="n">
-        <v>10</v>
-      </c>
-      <c r="O37" s="125" t="n">
-        <v>7</v>
-      </c>
-      <c r="P37" s="125" t="s">
-        <v>695</v>
-      </c>
-      <c r="Q37" s="125" t="n">
-        <v>5</v>
-      </c>
-      <c r="R37" s="125" t="n">
-        <v>11</v>
-      </c>
-      <c r="S37" s="125" t="n">
-        <v>6</v>
-      </c>
-      <c r="T37" s="125" t="n">
-        <v>11</v>
-      </c>
-      <c r="U37" s="125" t="n">
-        <v>5</v>
-      </c>
-      <c r="V37" s="125" t="n">
-        <v>2</v>
-      </c>
-      <c r="W37" s="126"/>
-      <c r="X37" s="126"/>
-      <c r="Y37" s="126"/>
-      <c r="Z37" s="126"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="124" t="s">
-        <v>355</v>
+        <v>286</v>
       </c>
       <c r="B38" s="125" t="n">
-        <f aca="false">COUNTIF(G32:BA32,"&lt;&gt;")</f>
-        <v>20</v>
+        <f aca="false">COUNTIF(G38:BA38,"&lt;&gt;")</f>
+        <v>17</v>
       </c>
       <c r="C38" s="125" t="n">
-        <f aca="false">COUNTIF(G32:BB32,"1")</f>
+        <f aca="false">COUNTIF(G38:BB38,"1")</f>
         <v>0</v>
       </c>
       <c r="D38" s="125" t="n">
-        <f aca="false">COUNTIF(G32:BC32,"2")</f>
-        <v>0</v>
+        <f aca="false">COUNTIF(G38:BC38,"2")</f>
+        <v>2</v>
       </c>
       <c r="E38" s="125" t="n">
-        <f aca="false">COUNTIF(G32:BD32,"3")</f>
-        <v>0</v>
+        <f aca="false">COUNTIF(G38:BD38,"3")</f>
+        <v>2</v>
       </c>
       <c r="F38" s="125" t="n">
-        <f aca="false">COUNTIF(G32:BC32,"*last*")</f>
-        <v>0</v>
+        <f aca="false">COUNTIF(G38:BC38,"*last*")</f>
+        <v>1</v>
       </c>
       <c r="G38" s="125" t="n">
+        <v>2</v>
+      </c>
+      <c r="H38" s="125" t="n">
+        <v>2</v>
+      </c>
+      <c r="I38" s="125" t="n">
+        <v>6</v>
+      </c>
+      <c r="J38" s="125" t="n">
+        <v>3</v>
+      </c>
+      <c r="K38" s="125" t="n">
+        <v>3</v>
+      </c>
+      <c r="L38" s="125" t="n">
+        <v>6</v>
+      </c>
+      <c r="M38" s="125" t="n">
+        <v>8</v>
+      </c>
+      <c r="N38" s="125" t="n">
         <v>4</v>
       </c>
-      <c r="H38" s="125" t="n">
-        <v>3</v>
-      </c>
-      <c r="I38" s="127"/>
-      <c r="J38" s="128" t="n">
+      <c r="O38" s="125" t="n">
+        <v>4</v>
+      </c>
+      <c r="P38" s="128"/>
+      <c r="Q38" s="125" t="s">
+        <v>698</v>
+      </c>
+      <c r="R38" s="125" t="n">
+        <v>13</v>
+      </c>
+      <c r="S38" s="125" t="n">
+        <v>8</v>
+      </c>
+      <c r="T38" s="125" t="n">
+        <v>6</v>
+      </c>
+      <c r="U38" s="125"/>
+      <c r="V38" s="125"/>
+      <c r="W38" s="125" t="n">
         <v>11</v>
       </c>
-      <c r="K38" s="125" t="n">
-        <v>6</v>
-      </c>
-      <c r="L38" s="125" t="n">
+      <c r="X38" s="125" t="n">
+        <v>9</v>
+      </c>
+      <c r="Y38" s="125" t="n">
         <v>7</v>
       </c>
-      <c r="M38" s="125" t="n">
-        <v>2</v>
-      </c>
-      <c r="N38" s="125" t="n">
-        <v>3</v>
-      </c>
-      <c r="O38" s="125" t="n">
-        <v>5</v>
-      </c>
-      <c r="P38" s="125" t="n">
-        <v>6</v>
-      </c>
-      <c r="Q38" s="125" t="n">
-        <v>8</v>
-      </c>
-      <c r="R38" s="125" t="n">
-        <v>1</v>
-      </c>
-      <c r="S38" s="125" t="n">
-        <v>11</v>
-      </c>
-      <c r="T38" s="125" t="n">
-        <v>1</v>
-      </c>
-      <c r="U38" s="125" t="n">
+      <c r="Z38" s="125" t="n">
         <v>12</v>
-      </c>
-      <c r="V38" s="125" t="n">
-        <v>7</v>
-      </c>
-      <c r="W38" s="125" t="n">
-        <v>4</v>
-      </c>
-      <c r="X38" s="125" t="n">
-        <v>5</v>
-      </c>
-      <c r="Y38" s="125" t="s">
-        <v>696</v>
-      </c>
-      <c r="Z38" s="125" t="n">
-        <v>9</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="124" t="s">
-        <v>286</v>
+        <v>313</v>
       </c>
       <c r="B39" s="125" t="n">
-        <f aca="false">COUNTIF(G33:BA33,"&lt;&gt;")</f>
-        <v>20</v>
+        <f aca="false">COUNTIF(G39:BA39,"&lt;&gt;")</f>
+        <v>16</v>
       </c>
       <c r="C39" s="125" t="n">
-        <f aca="false">COUNTIF(G33:BB33,"1")</f>
+        <f aca="false">COUNTIF(G39:BB39,"1")</f>
+        <v>0</v>
+      </c>
+      <c r="D39" s="125" t="n">
+        <f aca="false">COUNTIF(G39:BC39,"2")</f>
+        <v>1</v>
+      </c>
+      <c r="E39" s="125" t="n">
+        <f aca="false">COUNTIF(G39:BD39,"3")</f>
+        <v>0</v>
+      </c>
+      <c r="F39" s="125" t="n">
+        <f aca="false">COUNTIF(G39:BC39,"*last*")</f>
+        <v>1</v>
+      </c>
+      <c r="G39" s="125" t="n">
+        <v>10</v>
+      </c>
+      <c r="H39" s="125" t="n">
+        <v>8</v>
+      </c>
+      <c r="I39" s="125" t="n">
+        <v>8</v>
+      </c>
+      <c r="J39" s="125" t="n">
+        <v>4</v>
+      </c>
+      <c r="K39" s="125" t="n">
+        <v>10</v>
+      </c>
+      <c r="L39" s="125" t="n">
+        <v>10</v>
+      </c>
+      <c r="M39" s="125" t="n">
+        <v>9</v>
+      </c>
+      <c r="N39" s="125" t="n">
+        <v>10</v>
+      </c>
+      <c r="O39" s="125" t="n">
+        <v>7</v>
+      </c>
+      <c r="P39" s="125" t="s">
+        <v>696</v>
+      </c>
+      <c r="Q39" s="125" t="n">
+        <v>5</v>
+      </c>
+      <c r="R39" s="125" t="n">
+        <v>11</v>
+      </c>
+      <c r="S39" s="125" t="n">
+        <v>6</v>
+      </c>
+      <c r="T39" s="125" t="n">
+        <v>11</v>
+      </c>
+      <c r="U39" s="125" t="n">
+        <v>5</v>
+      </c>
+      <c r="V39" s="125" t="n">
         <v>2</v>
       </c>
-      <c r="D39" s="125" t="n">
-        <f aca="false">COUNTIF(G33:BC33,"2")</f>
-        <v>3</v>
-      </c>
-      <c r="E39" s="125" t="n">
-        <f aca="false">COUNTIF(G33:BD33,"3")</f>
-        <v>1</v>
-      </c>
-      <c r="F39" s="125" t="n">
-        <f aca="false">COUNTIF(G33:BC33,"*last*")</f>
-        <v>0</v>
-      </c>
-      <c r="G39" s="125" t="n">
-        <v>2</v>
-      </c>
-      <c r="H39" s="125" t="n">
-        <v>2</v>
-      </c>
-      <c r="I39" s="125" t="n">
-        <v>6</v>
-      </c>
-      <c r="J39" s="125" t="n">
-        <v>3</v>
-      </c>
-      <c r="K39" s="125" t="n">
-        <v>3</v>
-      </c>
-      <c r="L39" s="125" t="n">
-        <v>6</v>
-      </c>
-      <c r="M39" s="125" t="n">
-        <v>8</v>
-      </c>
-      <c r="N39" s="125" t="n">
-        <v>4</v>
-      </c>
-      <c r="O39" s="125" t="n">
-        <v>4</v>
-      </c>
-      <c r="P39" s="126"/>
-      <c r="Q39" s="125" t="s">
-        <v>697</v>
-      </c>
-      <c r="R39" s="125" t="n">
-        <v>13</v>
-      </c>
-      <c r="S39" s="125" t="n">
-        <v>8</v>
-      </c>
-      <c r="T39" s="125" t="n">
-        <v>6</v>
-      </c>
-      <c r="U39" s="125"/>
-      <c r="V39" s="125"/>
-      <c r="W39" s="125" t="n">
-        <v>11</v>
-      </c>
-      <c r="X39" s="125" t="n">
-        <v>9</v>
-      </c>
-      <c r="Y39" s="125" t="n">
-        <v>7</v>
-      </c>
-      <c r="Z39" s="125" t="n">
-        <v>12</v>
-      </c>
+      <c r="W39" s="128"/>
+      <c r="X39" s="128"/>
+      <c r="Y39" s="128"/>
+      <c r="Z39" s="128"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="124" t="s">
         <v>175</v>
       </c>
       <c r="B40" s="125" t="n">
-        <f aca="false">COUNTIF(G34:BA34,"&lt;&gt;")</f>
-        <v>20</v>
+        <f aca="false">COUNTIF(G40:BA40,"&lt;&gt;")</f>
+        <v>16</v>
       </c>
       <c r="C40" s="125" t="n">
-        <f aca="false">COUNTIF(G34:BB34,"1")</f>
-        <v>9</v>
+        <f aca="false">COUNTIF(G40:BB40,"1")</f>
+        <v>0</v>
       </c>
       <c r="D40" s="125" t="n">
-        <f aca="false">COUNTIF(G34:BC34,"2")</f>
-        <v>5</v>
+        <f aca="false">COUNTIF(G40:BC40,"2")</f>
+        <v>0</v>
       </c>
       <c r="E40" s="125" t="n">
-        <f aca="false">COUNTIF(G34:BD34,"3")</f>
-        <v>3</v>
+        <f aca="false">COUNTIF(G40:BD40,"3")</f>
+        <v>2</v>
       </c>
       <c r="F40" s="125" t="n">
-        <f aca="false">COUNTIF(G34:BC34,"*last*")</f>
-        <v>0</v>
-      </c>
-      <c r="G40" s="126"/>
-      <c r="H40" s="126"/>
-      <c r="I40" s="126"/>
-      <c r="J40" s="126"/>
+        <f aca="false">COUNTIF(G40:BC40,"*last*")</f>
+        <v>4</v>
+      </c>
+      <c r="G40" s="128"/>
+      <c r="H40" s="128"/>
+      <c r="I40" s="128"/>
+      <c r="J40" s="128"/>
       <c r="K40" s="125" t="s">
         <v>699</v>
       </c>
@@ -13027,13 +13025,13 @@
         <v>9</v>
       </c>
       <c r="U40" s="125" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="V40" s="125" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="W40" s="125" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="X40" s="125" t="n">
         <v>8</v>
@@ -13050,29 +13048,29 @@
         <v>219</v>
       </c>
       <c r="B41" s="125" t="n">
-        <f aca="false">COUNTIF(G35:BA35,"&lt;&gt;")</f>
-        <v>20</v>
+        <f aca="false">COUNTIF(G41:BA41,"&lt;&gt;")</f>
+        <v>15</v>
       </c>
       <c r="C41" s="125" t="n">
-        <f aca="false">COUNTIF(G35:BB35,"1")</f>
-        <v>1</v>
+        <f aca="false">COUNTIF(G41:BB41,"1")</f>
+        <v>0</v>
       </c>
       <c r="D41" s="125" t="n">
-        <f aca="false">COUNTIF(G35:BC35,"2")</f>
+        <f aca="false">COUNTIF(G41:BC41,"2")</f>
         <v>0</v>
       </c>
       <c r="E41" s="125" t="n">
-        <f aca="false">COUNTIF(G35:BD35,"3")</f>
-        <v>2</v>
+        <f aca="false">COUNTIF(G41:BD41,"3")</f>
+        <v>0</v>
       </c>
       <c r="F41" s="125" t="n">
-        <f aca="false">COUNTIF(G35:BC35,"*last*")</f>
-        <v>3</v>
-      </c>
-      <c r="G41" s="126"/>
-      <c r="H41" s="126"/>
-      <c r="I41" s="126"/>
-      <c r="J41" s="126"/>
+        <f aca="false">COUNTIF(G41:BC41,"*last*")</f>
+        <v>0</v>
+      </c>
+      <c r="G41" s="128"/>
+      <c r="H41" s="128"/>
+      <c r="I41" s="128"/>
+      <c r="J41" s="128"/>
       <c r="K41" s="125" t="n">
         <v>4</v>
       </c>
@@ -13082,7 +13080,7 @@
       <c r="M41" s="125" t="n">
         <v>10</v>
       </c>
-      <c r="N41" s="126"/>
+      <c r="N41" s="128"/>
       <c r="O41" s="125" t="n">
         <v>10</v>
       </c>
@@ -13125,31 +13123,31 @@
         <v>201</v>
       </c>
       <c r="B42" s="125" t="n">
-        <f aca="false">COUNTIF(G36:BA36,"&lt;&gt;")</f>
-        <v>20</v>
+        <f aca="false">COUNTIF(G42:BA42,"&lt;&gt;")</f>
+        <v>14</v>
       </c>
       <c r="C42" s="125" t="n">
-        <f aca="false">COUNTIF(G36:BB36,"1")</f>
-        <v>2</v>
+        <f aca="false">COUNTIF(G42:BB42,"1")</f>
+        <v>0</v>
       </c>
       <c r="D42" s="125" t="n">
-        <f aca="false">COUNTIF(G36:BC36,"2")</f>
-        <v>2</v>
+        <f aca="false">COUNTIF(G42:BC42,"2")</f>
+        <v>1</v>
       </c>
       <c r="E42" s="125" t="n">
-        <f aca="false">COUNTIF(G36:BD36,"3")</f>
-        <v>4</v>
+        <f aca="false">COUNTIF(G42:BD42,"3")</f>
+        <v>1</v>
       </c>
       <c r="F42" s="125" t="n">
-        <f aca="false">COUNTIF(G36:BC36,"*last*")</f>
-        <v>1</v>
-      </c>
-      <c r="G42" s="126"/>
-      <c r="H42" s="126"/>
-      <c r="I42" s="126"/>
-      <c r="J42" s="126"/>
-      <c r="K42" s="126"/>
-      <c r="L42" s="126"/>
+        <f aca="false">COUNTIF(G42:BC42,"*last*")</f>
+        <v>0</v>
+      </c>
+      <c r="G42" s="128"/>
+      <c r="H42" s="128"/>
+      <c r="I42" s="128"/>
+      <c r="J42" s="128"/>
+      <c r="K42" s="128"/>
+      <c r="L42" s="128"/>
       <c r="M42" s="125" t="n">
         <v>11</v>
       </c>
@@ -13198,34 +13196,34 @@
         <v>236</v>
       </c>
       <c r="B43" s="125" t="n">
-        <f aca="false">COUNTIF(G37:BA37,"&lt;&gt;")</f>
-        <v>16</v>
+        <f aca="false">COUNTIF(G43:BA43,"&lt;&gt;")</f>
+        <v>11</v>
       </c>
       <c r="C43" s="125" t="n">
-        <f aca="false">COUNTIF(G37:BB37,"1")</f>
+        <f aca="false">COUNTIF(G43:BB43,"1")</f>
         <v>0</v>
       </c>
       <c r="D43" s="125" t="n">
-        <f aca="false">COUNTIF(G37:BC37,"2")</f>
-        <v>1</v>
+        <f aca="false">COUNTIF(G43:BC43,"2")</f>
+        <v>0</v>
       </c>
       <c r="E43" s="125" t="n">
-        <f aca="false">COUNTIF(G37:BD37,"3")</f>
+        <f aca="false">COUNTIF(G43:BD43,"3")</f>
+        <v>1</v>
+      </c>
+      <c r="F43" s="125" t="n">
+        <f aca="false">COUNTIF(G43:BC43,"*last*")</f>
         <v>0</v>
       </c>
-      <c r="F43" s="125" t="n">
-        <f aca="false">COUNTIF(G37:BC37,"*last*")</f>
-        <v>1</v>
-      </c>
-      <c r="G43" s="126"/>
-      <c r="H43" s="126"/>
-      <c r="I43" s="126"/>
-      <c r="J43" s="126"/>
-      <c r="K43" s="126"/>
-      <c r="L43" s="126"/>
-      <c r="M43" s="126"/>
-      <c r="N43" s="126"/>
-      <c r="O43" s="126"/>
+      <c r="G43" s="128"/>
+      <c r="H43" s="128"/>
+      <c r="I43" s="128"/>
+      <c r="J43" s="128"/>
+      <c r="K43" s="128"/>
+      <c r="L43" s="128"/>
+      <c r="M43" s="128"/>
+      <c r="N43" s="128"/>
+      <c r="O43" s="128"/>
       <c r="P43" s="125" t="n">
         <v>10</v>
       </c>
@@ -13265,24 +13263,24 @@
         <v>341</v>
       </c>
       <c r="B44" s="125" t="n">
-        <f aca="false">COUNTIF(G38:BA38,"&lt;&gt;")</f>
-        <v>19</v>
+        <f aca="false">COUNTIF(G44:BA44,"&lt;&gt;")</f>
+        <v>8</v>
       </c>
       <c r="C44" s="125" t="n">
-        <f aca="false">COUNTIF(G38:BB38,"1")</f>
-        <v>2</v>
+        <f aca="false">COUNTIF(G44:BB44,"1")</f>
+        <v>1</v>
       </c>
       <c r="D44" s="125" t="n">
-        <f aca="false">COUNTIF(G38:BC38,"2")</f>
-        <v>1</v>
+        <f aca="false">COUNTIF(G44:BC44,"2")</f>
+        <v>0</v>
       </c>
       <c r="E44" s="125" t="n">
-        <f aca="false">COUNTIF(G38:BD38,"3")</f>
-        <v>2</v>
+        <f aca="false">COUNTIF(G44:BD44,"3")</f>
+        <v>1</v>
       </c>
       <c r="F44" s="125" t="n">
-        <f aca="false">COUNTIF(G38:BC38,"*last*")</f>
-        <v>1</v>
+        <f aca="false">COUNTIF(G44:BC44,"*last*")</f>
+        <v>0</v>
       </c>
       <c r="G44" s="125" t="n">
         <v>8</v>
@@ -13308,51 +13306,51 @@
       <c r="N44" s="125" t="n">
         <v>9</v>
       </c>
-      <c r="O44" s="126"/>
-      <c r="P44" s="126"/>
-      <c r="Q44" s="126"/>
-      <c r="R44" s="126"/>
-      <c r="S44" s="126"/>
-      <c r="T44" s="126"/>
-      <c r="U44" s="126"/>
-      <c r="V44" s="126"/>
-      <c r="W44" s="126"/>
-      <c r="X44" s="126"/>
-      <c r="Y44" s="126"/>
-      <c r="Z44" s="126"/>
+      <c r="O44" s="128"/>
+      <c r="P44" s="128"/>
+      <c r="Q44" s="128"/>
+      <c r="R44" s="128"/>
+      <c r="S44" s="128"/>
+      <c r="T44" s="128"/>
+      <c r="U44" s="128"/>
+      <c r="V44" s="128"/>
+      <c r="W44" s="128"/>
+      <c r="X44" s="128"/>
+      <c r="Y44" s="128"/>
+      <c r="Z44" s="128"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="124" t="s">
         <v>322</v>
       </c>
       <c r="B45" s="125" t="n">
-        <f aca="false">COUNTIF(G39:BA39,"&lt;&gt;")</f>
-        <v>17</v>
+        <f aca="false">COUNTIF(G45:BA45,"&lt;&gt;")</f>
+        <v>7</v>
       </c>
       <c r="C45" s="125" t="n">
-        <f aca="false">COUNTIF(G39:BB39,"1")</f>
+        <f aca="false">COUNTIF(G45:BB45,"1")</f>
         <v>0</v>
       </c>
       <c r="D45" s="125" t="n">
-        <f aca="false">COUNTIF(G39:BC39,"2")</f>
+        <f aca="false">COUNTIF(G45:BC45,"2")</f>
         <v>2</v>
       </c>
       <c r="E45" s="125" t="n">
-        <f aca="false">COUNTIF(G39:BD39,"3")</f>
-        <v>2</v>
+        <f aca="false">COUNTIF(G45:BD45,"3")</f>
+        <v>0</v>
       </c>
       <c r="F45" s="125" t="n">
-        <f aca="false">COUNTIF(G39:BC39,"*last*")</f>
-        <v>1</v>
-      </c>
-      <c r="G45" s="126"/>
-      <c r="H45" s="126"/>
-      <c r="I45" s="126"/>
-      <c r="J45" s="126"/>
-      <c r="K45" s="126"/>
-      <c r="L45" s="126"/>
-      <c r="M45" s="126"/>
-      <c r="N45" s="126"/>
+        <f aca="false">COUNTIF(G45:BC45,"*last*")</f>
+        <v>1</v>
+      </c>
+      <c r="G45" s="128"/>
+      <c r="H45" s="128"/>
+      <c r="I45" s="128"/>
+      <c r="J45" s="128"/>
+      <c r="K45" s="128"/>
+      <c r="L45" s="128"/>
+      <c r="M45" s="128"/>
+      <c r="N45" s="128"/>
       <c r="O45" s="125" t="n">
         <v>2</v>
       </c>
@@ -13369,49 +13367,49 @@
         <v>10</v>
       </c>
       <c r="T45" s="125" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="U45" s="125" t="n">
         <v>10</v>
       </c>
-      <c r="V45" s="126"/>
-      <c r="W45" s="126"/>
-      <c r="X45" s="126"/>
-      <c r="Y45" s="126"/>
-      <c r="Z45" s="126"/>
+      <c r="V45" s="128"/>
+      <c r="W45" s="128"/>
+      <c r="X45" s="128"/>
+      <c r="Y45" s="128"/>
+      <c r="Z45" s="128"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="124" t="s">
         <v>338</v>
       </c>
       <c r="B46" s="125" t="n">
-        <f aca="false">COUNTIF(G40:BA40,"&lt;&gt;")</f>
-        <v>16</v>
+        <f aca="false">COUNTIF(G46:BA46,"&lt;&gt;")</f>
+        <v>7</v>
       </c>
       <c r="C46" s="125" t="n">
-        <f aca="false">COUNTIF(G40:BB40,"1")</f>
+        <f aca="false">COUNTIF(G46:BB46,"1")</f>
         <v>0</v>
       </c>
       <c r="D46" s="125" t="n">
-        <f aca="false">COUNTIF(G40:BC40,"2")</f>
+        <f aca="false">COUNTIF(G46:BC46,"2")</f>
         <v>0</v>
       </c>
       <c r="E46" s="125" t="n">
-        <f aca="false">COUNTIF(G40:BD40,"3")</f>
-        <v>2</v>
+        <f aca="false">COUNTIF(G46:BD46,"3")</f>
+        <v>0</v>
       </c>
       <c r="F46" s="125" t="n">
-        <f aca="false">COUNTIF(G40:BC40,"*last*")</f>
-        <v>4</v>
-      </c>
-      <c r="G46" s="126"/>
-      <c r="H46" s="126"/>
-      <c r="I46" s="126"/>
-      <c r="J46" s="126"/>
-      <c r="K46" s="126"/>
-      <c r="L46" s="126"/>
+        <f aca="false">COUNTIF(G46:BC46,"*last*")</f>
+        <v>1</v>
+      </c>
+      <c r="G46" s="128"/>
+      <c r="H46" s="128"/>
+      <c r="I46" s="128"/>
+      <c r="J46" s="128"/>
+      <c r="K46" s="128"/>
+      <c r="L46" s="128"/>
       <c r="M46" s="125" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="N46" s="125" t="n">
         <v>12</v>
@@ -13419,13 +13417,13 @@
       <c r="O46" s="125" t="n">
         <v>8</v>
       </c>
-      <c r="P46" s="126"/>
+      <c r="P46" s="128"/>
       <c r="Q46" s="125" t="n">
         <v>10</v>
       </c>
-      <c r="R46" s="126"/>
-      <c r="S46" s="126"/>
-      <c r="T46" s="126"/>
+      <c r="R46" s="128"/>
+      <c r="S46" s="128"/>
+      <c r="T46" s="128"/>
       <c r="U46" s="125" t="n">
         <v>4</v>
       </c>
@@ -13435,670 +13433,670 @@
       <c r="W46" s="125" t="n">
         <v>10</v>
       </c>
-      <c r="X46" s="126"/>
-      <c r="Y46" s="126"/>
-      <c r="Z46" s="126"/>
+      <c r="X46" s="128"/>
+      <c r="Y46" s="128"/>
+      <c r="Z46" s="128"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="124" t="s">
-        <v>681</v>
+        <v>261</v>
       </c>
       <c r="B47" s="125" t="n">
-        <f aca="false">COUNTIF(G41:BA41,"&lt;&gt;")</f>
-        <v>15</v>
+        <f aca="false">COUNTIF(G47:BA47,"&lt;&gt;")</f>
+        <v>6</v>
       </c>
       <c r="C47" s="125" t="n">
-        <f aca="false">COUNTIF(G41:BB41,"1")</f>
+        <f aca="false">COUNTIF(G47:BB47,"1")</f>
+        <v>3</v>
+      </c>
+      <c r="D47" s="125" t="n">
+        <f aca="false">COUNTIF(G47:BC47,"2")</f>
+        <v>1</v>
+      </c>
+      <c r="E47" s="125" t="n">
+        <f aca="false">COUNTIF(G47:BD47,"3")</f>
         <v>0</v>
       </c>
-      <c r="D47" s="125" t="n">
-        <f aca="false">COUNTIF(G41:BC41,"2")</f>
+      <c r="F47" s="125" t="n">
+        <f aca="false">COUNTIF(G47:BC47,"*last*")</f>
         <v>0</v>
       </c>
-      <c r="E47" s="125" t="n">
-        <f aca="false">COUNTIF(G41:BD41,"3")</f>
-        <v>0</v>
-      </c>
-      <c r="F47" s="125" t="n">
-        <f aca="false">COUNTIF(G41:BC41,"*last*")</f>
-        <v>0</v>
-      </c>
-      <c r="G47" s="125" t="n">
-        <v>6</v>
-      </c>
-      <c r="H47" s="125" t="n">
-        <v>5</v>
-      </c>
-      <c r="I47" s="125" t="n">
-        <v>3</v>
-      </c>
-      <c r="J47" s="125" t="n">
-        <v>5</v>
-      </c>
-      <c r="K47" s="125" t="n">
+      <c r="G47" s="128"/>
+      <c r="H47" s="128"/>
+      <c r="I47" s="128"/>
+      <c r="J47" s="128"/>
+      <c r="K47" s="128"/>
+      <c r="L47" s="128"/>
+      <c r="M47" s="128"/>
+      <c r="N47" s="128"/>
+      <c r="O47" s="128"/>
+      <c r="P47" s="128"/>
+      <c r="Q47" s="128"/>
+      <c r="R47" s="128"/>
+      <c r="S47" s="128"/>
+      <c r="T47" s="128"/>
+      <c r="U47" s="125" t="n">
         <v>2</v>
       </c>
-      <c r="L47" s="125" t="s">
-        <v>699</v>
-      </c>
-      <c r="M47" s="127"/>
-      <c r="N47" s="127"/>
-      <c r="O47" s="126"/>
-      <c r="P47" s="126"/>
-      <c r="Q47" s="126"/>
-      <c r="R47" s="126"/>
-      <c r="S47" s="126"/>
-      <c r="T47" s="126"/>
-      <c r="U47" s="126"/>
-      <c r="V47" s="126"/>
-      <c r="W47" s="126"/>
-      <c r="X47" s="126"/>
-      <c r="Y47" s="126"/>
-      <c r="Z47" s="126"/>
+      <c r="V47" s="125" t="n">
+        <v>4</v>
+      </c>
+      <c r="W47" s="125" t="n">
+        <v>1</v>
+      </c>
+      <c r="X47" s="125" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y47" s="125" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z47" s="125" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="124" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B48" s="125" t="n">
-        <f aca="false">COUNTIF(G42:BA42,"&lt;&gt;")</f>
-        <v>14</v>
+        <f aca="false">COUNTIF(G48:BA48,"&lt;&gt;")</f>
+        <v>6</v>
       </c>
       <c r="C48" s="125" t="n">
-        <f aca="false">COUNTIF(G42:BB42,"1")</f>
+        <f aca="false">COUNTIF(G48:BB48,"1")</f>
         <v>0</v>
       </c>
       <c r="D48" s="125" t="n">
-        <f aca="false">COUNTIF(G42:BC42,"2")</f>
+        <f aca="false">COUNTIF(G48:BC48,"2")</f>
         <v>1</v>
       </c>
       <c r="E48" s="125" t="n">
-        <f aca="false">COUNTIF(G42:BD42,"3")</f>
+        <f aca="false">COUNTIF(G48:BD48,"3")</f>
         <v>1</v>
       </c>
       <c r="F48" s="125" t="n">
-        <f aca="false">COUNTIF(G42:BC42,"*last*")</f>
-        <v>0</v>
+        <f aca="false">COUNTIF(G48:BC48,"*last*")</f>
+        <v>1</v>
       </c>
       <c r="G48" s="125" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H48" s="125" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I48" s="125" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="J48" s="125" t="n">
-        <v>9</v>
-      </c>
-      <c r="K48" s="126"/>
-      <c r="L48" s="126"/>
+        <v>5</v>
+      </c>
+      <c r="K48" s="125" t="n">
+        <v>2</v>
+      </c>
+      <c r="L48" s="125" t="s">
+        <v>699</v>
+      </c>
       <c r="M48" s="126"/>
       <c r="N48" s="126"/>
-      <c r="O48" s="126"/>
-      <c r="P48" s="126"/>
-      <c r="Q48" s="126"/>
-      <c r="R48" s="126"/>
-      <c r="S48" s="126"/>
-      <c r="T48" s="126"/>
-      <c r="U48" s="126"/>
-      <c r="V48" s="126"/>
-      <c r="W48" s="126"/>
-      <c r="X48" s="126"/>
-      <c r="Y48" s="126"/>
-      <c r="Z48" s="126"/>
+      <c r="O48" s="128"/>
+      <c r="P48" s="128"/>
+      <c r="Q48" s="128"/>
+      <c r="R48" s="128"/>
+      <c r="S48" s="128"/>
+      <c r="T48" s="128"/>
+      <c r="U48" s="128"/>
+      <c r="V48" s="128"/>
+      <c r="W48" s="128"/>
+      <c r="X48" s="128"/>
+      <c r="Y48" s="128"/>
+      <c r="Z48" s="128"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="124" t="s">
-        <v>688</v>
+        <v>275</v>
       </c>
       <c r="B49" s="125" t="n">
-        <f aca="false">COUNTIF(G43:BA43,"&lt;&gt;")</f>
-        <v>11</v>
+        <f aca="false">COUNTIF(G49:BA49,"&lt;&gt;")</f>
+        <v>5</v>
       </c>
       <c r="C49" s="125" t="n">
-        <f aca="false">COUNTIF(G43:BB43,"1")</f>
+        <f aca="false">COUNTIF(G49:BB49,"1")</f>
         <v>0</v>
       </c>
       <c r="D49" s="125" t="n">
-        <f aca="false">COUNTIF(G43:BC43,"2")</f>
+        <f aca="false">COUNTIF(G49:BC49,"2")</f>
         <v>0</v>
       </c>
       <c r="E49" s="125" t="n">
-        <f aca="false">COUNTIF(G43:BD43,"3")</f>
-        <v>1</v>
+        <f aca="false">COUNTIF(G49:BD49,"3")</f>
+        <v>0</v>
       </c>
       <c r="F49" s="125" t="n">
-        <f aca="false">COUNTIF(G43:BC43,"*last*")</f>
-        <v>0</v>
-      </c>
-      <c r="G49" s="126"/>
-      <c r="H49" s="126"/>
-      <c r="I49" s="126"/>
-      <c r="J49" s="126"/>
-      <c r="K49" s="126"/>
-      <c r="L49" s="126"/>
-      <c r="M49" s="126"/>
-      <c r="N49" s="126"/>
-      <c r="O49" s="126"/>
-      <c r="P49" s="125" t="n">
+        <f aca="false">COUNTIF(G49:BC49,"*last*")</f>
+        <v>1</v>
+      </c>
+      <c r="G49" s="128"/>
+      <c r="H49" s="128"/>
+      <c r="I49" s="128"/>
+      <c r="J49" s="128"/>
+      <c r="K49" s="128"/>
+      <c r="L49" s="128"/>
+      <c r="M49" s="128"/>
+      <c r="N49" s="128"/>
+      <c r="O49" s="128"/>
+      <c r="P49" s="128"/>
+      <c r="Q49" s="128"/>
+      <c r="R49" s="128"/>
+      <c r="S49" s="128"/>
+      <c r="T49" s="128"/>
+      <c r="U49" s="128"/>
+      <c r="V49" s="125" t="n">
+        <v>6</v>
+      </c>
+      <c r="W49" s="125" t="n">
+        <v>6</v>
+      </c>
+      <c r="X49" s="125" t="s">
+        <v>700</v>
+      </c>
+      <c r="Y49" s="125" t="n">
+        <v>6</v>
+      </c>
+      <c r="Z49" s="125" t="n">
         <v>7</v>
       </c>
-      <c r="Q49" s="125" t="n">
-        <v>13</v>
-      </c>
-      <c r="R49" s="125" t="n">
-        <v>9</v>
-      </c>
-      <c r="S49" s="125" t="s">
-        <v>697</v>
-      </c>
-      <c r="T49" s="126"/>
-      <c r="U49" s="126"/>
-      <c r="V49" s="126"/>
-      <c r="W49" s="126"/>
-      <c r="X49" s="126"/>
-      <c r="Y49" s="126"/>
-      <c r="Z49" s="126"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="124" t="s">
-        <v>261</v>
+        <v>688</v>
       </c>
       <c r="B50" s="125" t="n">
-        <f aca="false">COUNTIF(G44:BA44,"&lt;&gt;")</f>
-        <v>8</v>
+        <f aca="false">COUNTIF(G50:BA50,"&lt;&gt;")</f>
+        <v>4</v>
       </c>
       <c r="C50" s="125" t="n">
-        <f aca="false">COUNTIF(G44:BB44,"1")</f>
-        <v>1</v>
+        <f aca="false">COUNTIF(G50:BB50,"1")</f>
+        <v>0</v>
       </c>
       <c r="D50" s="125" t="n">
-        <f aca="false">COUNTIF(G44:BC44,"2")</f>
+        <f aca="false">COUNTIF(G50:BC50,"2")</f>
         <v>0</v>
       </c>
       <c r="E50" s="125" t="n">
-        <f aca="false">COUNTIF(G44:BD44,"3")</f>
-        <v>1</v>
+        <f aca="false">COUNTIF(G50:BD50,"3")</f>
+        <v>0</v>
       </c>
       <c r="F50" s="125" t="n">
-        <f aca="false">COUNTIF(G44:BC44,"*last*")</f>
-        <v>0</v>
-      </c>
-      <c r="G50" s="126"/>
-      <c r="H50" s="126"/>
-      <c r="I50" s="126"/>
-      <c r="J50" s="126"/>
-      <c r="K50" s="126"/>
-      <c r="L50" s="126"/>
-      <c r="M50" s="126"/>
-      <c r="N50" s="126"/>
-      <c r="O50" s="126"/>
-      <c r="P50" s="126"/>
-      <c r="Q50" s="126"/>
-      <c r="R50" s="126"/>
-      <c r="S50" s="126"/>
-      <c r="T50" s="126"/>
-      <c r="U50" s="125" t="n">
-        <v>2</v>
-      </c>
-      <c r="V50" s="125" t="n">
-        <v>4</v>
-      </c>
-      <c r="W50" s="125" t="n">
-        <v>1</v>
-      </c>
-      <c r="X50" s="125" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y50" s="125" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z50" s="125" t="n">
-        <v>4</v>
-      </c>
+        <f aca="false">COUNTIF(G50:BC50,"*last*")</f>
+        <v>1</v>
+      </c>
+      <c r="G50" s="128"/>
+      <c r="H50" s="128"/>
+      <c r="I50" s="128"/>
+      <c r="J50" s="128"/>
+      <c r="K50" s="128"/>
+      <c r="L50" s="128"/>
+      <c r="M50" s="128"/>
+      <c r="N50" s="128"/>
+      <c r="O50" s="128"/>
+      <c r="P50" s="125" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q50" s="125" t="n">
+        <v>13</v>
+      </c>
+      <c r="R50" s="125" t="n">
+        <v>9</v>
+      </c>
+      <c r="S50" s="125" t="s">
+        <v>698</v>
+      </c>
+      <c r="T50" s="128"/>
+      <c r="U50" s="128"/>
+      <c r="V50" s="128"/>
+      <c r="W50" s="128"/>
+      <c r="X50" s="128"/>
+      <c r="Y50" s="128"/>
+      <c r="Z50" s="128"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="124" t="s">
-        <v>334</v>
+        <v>682</v>
       </c>
       <c r="B51" s="125" t="n">
-        <f aca="false">COUNTIF(G45:BA45,"&lt;&gt;")</f>
+        <f aca="false">COUNTIF(G51:BA51,"&lt;&gt;")</f>
+        <v>4</v>
+      </c>
+      <c r="C51" s="125" t="n">
+        <f aca="false">COUNTIF(G51:BB51,"1")</f>
+        <v>0</v>
+      </c>
+      <c r="D51" s="125" t="n">
+        <f aca="false">COUNTIF(G51:BC51,"2")</f>
+        <v>0</v>
+      </c>
+      <c r="E51" s="125" t="n">
+        <f aca="false">COUNTIF(G51:BD51,"3")</f>
+        <v>0</v>
+      </c>
+      <c r="F51" s="125" t="n">
+        <f aca="false">COUNTIF(G51:BC51,"*last*")</f>
+        <v>0</v>
+      </c>
+      <c r="G51" s="125" t="n">
         <v>7</v>
       </c>
-      <c r="C51" s="125" t="n">
-        <f aca="false">COUNTIF(G45:BB45,"1")</f>
-        <v>0</v>
-      </c>
-      <c r="D51" s="125" t="n">
-        <f aca="false">COUNTIF(G45:BC45,"2")</f>
-        <v>2</v>
-      </c>
-      <c r="E51" s="125" t="n">
-        <f aca="false">COUNTIF(G45:BD45,"3")</f>
-        <v>0</v>
-      </c>
-      <c r="F51" s="125" t="n">
-        <f aca="false">COUNTIF(G45:BC45,"*last*")</f>
-        <v>1</v>
-      </c>
-      <c r="G51" s="126"/>
-      <c r="H51" s="126"/>
-      <c r="I51" s="126"/>
-      <c r="J51" s="126"/>
-      <c r="K51" s="126"/>
-      <c r="L51" s="126"/>
-      <c r="M51" s="125" t="n">
-        <v>12</v>
-      </c>
-      <c r="N51" s="125" t="n">
-        <v>11</v>
-      </c>
-      <c r="O51" s="125" t="n">
-        <v>12</v>
-      </c>
-      <c r="P51" s="126"/>
-      <c r="Q51" s="126"/>
-      <c r="R51" s="126"/>
-      <c r="S51" s="126"/>
-      <c r="T51" s="126"/>
-      <c r="U51" s="126"/>
-      <c r="V51" s="126"/>
-      <c r="W51" s="126"/>
-      <c r="X51" s="126"/>
-      <c r="Y51" s="126"/>
-      <c r="Z51" s="126"/>
+      <c r="H51" s="125" t="n">
+        <v>7</v>
+      </c>
+      <c r="I51" s="125" t="n">
+        <v>9</v>
+      </c>
+      <c r="J51" s="125" t="n">
+        <v>9</v>
+      </c>
+      <c r="K51" s="128"/>
+      <c r="L51" s="128"/>
+      <c r="M51" s="128"/>
+      <c r="N51" s="128"/>
+      <c r="O51" s="128"/>
+      <c r="P51" s="128"/>
+      <c r="Q51" s="128"/>
+      <c r="R51" s="128"/>
+      <c r="S51" s="128"/>
+      <c r="T51" s="128"/>
+      <c r="U51" s="128"/>
+      <c r="V51" s="128"/>
+      <c r="W51" s="128"/>
+      <c r="X51" s="128"/>
+      <c r="Y51" s="128"/>
+      <c r="Z51" s="128"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="124" t="s">
-        <v>345</v>
+        <v>251</v>
       </c>
       <c r="B52" s="125" t="n">
-        <f aca="false">COUNTIF(G46:BA46,"&lt;&gt;")</f>
-        <v>7</v>
+        <f aca="false">COUNTIF(G52:BA52,"&lt;&gt;")</f>
+        <v>3</v>
       </c>
       <c r="C52" s="125" t="n">
-        <f aca="false">COUNTIF(G46:BB46,"1")</f>
+        <f aca="false">COUNTIF(G52:BB52,"1")</f>
         <v>0</v>
       </c>
       <c r="D52" s="125" t="n">
-        <f aca="false">COUNTIF(G46:BC46,"2")</f>
+        <f aca="false">COUNTIF(G52:BC52,"2")</f>
         <v>0</v>
       </c>
       <c r="E52" s="125" t="n">
-        <f aca="false">COUNTIF(G46:BD46,"3")</f>
+        <f aca="false">COUNTIF(G52:BD52,"3")</f>
         <v>0</v>
       </c>
       <c r="F52" s="125" t="n">
-        <f aca="false">COUNTIF(G46:BC46,"*last*")</f>
-        <v>1</v>
-      </c>
-      <c r="G52" s="126"/>
-      <c r="H52" s="126"/>
-      <c r="I52" s="126"/>
-      <c r="J52" s="126"/>
-      <c r="K52" s="126"/>
-      <c r="L52" s="126"/>
-      <c r="M52" s="126"/>
-      <c r="N52" s="125" t="s">
-        <v>696</v>
-      </c>
-      <c r="O52" s="126"/>
-      <c r="P52" s="126"/>
-      <c r="Q52" s="126"/>
-      <c r="R52" s="125" t="n">
-        <v>10</v>
-      </c>
-      <c r="S52" s="125" t="n">
+        <f aca="false">COUNTIF(G52:BC52,"*last*")</f>
+        <v>1</v>
+      </c>
+      <c r="G52" s="128"/>
+      <c r="H52" s="128"/>
+      <c r="I52" s="128"/>
+      <c r="J52" s="128"/>
+      <c r="K52" s="128"/>
+      <c r="L52" s="128"/>
+      <c r="M52" s="128"/>
+      <c r="N52" s="128"/>
+      <c r="O52" s="128"/>
+      <c r="P52" s="128"/>
+      <c r="Q52" s="128"/>
+      <c r="R52" s="128"/>
+      <c r="S52" s="128"/>
+      <c r="T52" s="128"/>
+      <c r="U52" s="128"/>
+      <c r="V52" s="128"/>
+      <c r="W52" s="128"/>
+      <c r="X52" s="125" t="n">
         <v>12</v>
       </c>
-      <c r="T52" s="126"/>
-      <c r="U52" s="126"/>
-      <c r="V52" s="126"/>
-      <c r="W52" s="126"/>
-      <c r="X52" s="126"/>
-      <c r="Y52" s="126"/>
-      <c r="Z52" s="126"/>
+      <c r="Y52" s="125" t="n">
+        <v>9</v>
+      </c>
+      <c r="Z52" s="125" t="s">
+        <v>697</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="124" t="s">
-        <v>275</v>
+        <v>334</v>
       </c>
       <c r="B53" s="125" t="n">
-        <f aca="false">COUNTIF(G47:BA47,"&lt;&gt;")</f>
-        <v>6</v>
+        <f aca="false">COUNTIF(G53:BA53,"&lt;&gt;")</f>
+        <v>3</v>
       </c>
       <c r="C53" s="125" t="n">
-        <f aca="false">COUNTIF(G47:BB47,"1")</f>
+        <f aca="false">COUNTIF(G53:BB53,"1")</f>
         <v>0</v>
       </c>
       <c r="D53" s="125" t="n">
-        <f aca="false">COUNTIF(G47:BC47,"2")</f>
-        <v>1</v>
+        <f aca="false">COUNTIF(G53:BC53,"2")</f>
+        <v>0</v>
       </c>
       <c r="E53" s="125" t="n">
-        <f aca="false">COUNTIF(G47:BD47,"3")</f>
-        <v>1</v>
+        <f aca="false">COUNTIF(G53:BD53,"3")</f>
+        <v>0</v>
       </c>
       <c r="F53" s="125" t="n">
-        <f aca="false">COUNTIF(G47:BC47,"*last*")</f>
-        <v>1</v>
-      </c>
-      <c r="G53" s="126"/>
-      <c r="H53" s="126"/>
-      <c r="I53" s="126"/>
-      <c r="J53" s="126"/>
-      <c r="K53" s="126"/>
-      <c r="L53" s="126"/>
-      <c r="M53" s="126"/>
-      <c r="N53" s="126"/>
-      <c r="O53" s="126"/>
-      <c r="P53" s="126"/>
-      <c r="Q53" s="126"/>
-      <c r="R53" s="126"/>
-      <c r="S53" s="126"/>
-      <c r="T53" s="126"/>
-      <c r="U53" s="126"/>
-      <c r="V53" s="125" t="n">
-        <v>6</v>
-      </c>
-      <c r="W53" s="125" t="n">
-        <v>6</v>
-      </c>
-      <c r="X53" s="125" t="s">
-        <v>700</v>
-      </c>
-      <c r="Y53" s="125" t="n">
-        <v>6</v>
-      </c>
-      <c r="Z53" s="125" t="n">
-        <v>7</v>
-      </c>
+        <f aca="false">COUNTIF(G53:BC53,"*last*")</f>
+        <v>0</v>
+      </c>
+      <c r="G53" s="128"/>
+      <c r="H53" s="128"/>
+      <c r="I53" s="128"/>
+      <c r="J53" s="128"/>
+      <c r="K53" s="128"/>
+      <c r="L53" s="128"/>
+      <c r="M53" s="125" t="n">
+        <v>12</v>
+      </c>
+      <c r="N53" s="125" t="n">
+        <v>11</v>
+      </c>
+      <c r="O53" s="125" t="n">
+        <v>12</v>
+      </c>
+      <c r="P53" s="128"/>
+      <c r="Q53" s="128"/>
+      <c r="R53" s="128"/>
+      <c r="S53" s="128"/>
+      <c r="T53" s="128"/>
+      <c r="U53" s="128"/>
+      <c r="V53" s="128"/>
+      <c r="W53" s="128"/>
+      <c r="X53" s="128"/>
+      <c r="Y53" s="128"/>
+      <c r="Z53" s="128"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="124" t="s">
-        <v>684</v>
+        <v>345</v>
       </c>
       <c r="B54" s="125" t="n">
-        <f aca="false">COUNTIF(G48:BA48,"&lt;&gt;")</f>
-        <v>4</v>
+        <f aca="false">COUNTIF(G54:BA54,"&lt;&gt;")</f>
+        <v>3</v>
       </c>
       <c r="C54" s="125" t="n">
-        <f aca="false">COUNTIF(G48:BB48,"1")</f>
+        <f aca="false">COUNTIF(G54:BB54,"1")</f>
         <v>0</v>
       </c>
       <c r="D54" s="125" t="n">
-        <f aca="false">COUNTIF(G48:BC48,"2")</f>
+        <f aca="false">COUNTIF(G54:BC54,"2")</f>
         <v>0</v>
       </c>
       <c r="E54" s="125" t="n">
-        <f aca="false">COUNTIF(G48:BD48,"3")</f>
+        <f aca="false">COUNTIF(G54:BD54,"3")</f>
         <v>0</v>
       </c>
       <c r="F54" s="125" t="n">
-        <f aca="false">COUNTIF(G48:BC48,"*last*")</f>
-        <v>0</v>
-      </c>
-      <c r="G54" s="127"/>
-      <c r="H54" s="125" t="n">
-        <v>9</v>
-      </c>
-      <c r="I54" s="125" t="n">
-        <v>2</v>
-      </c>
-      <c r="J54" s="126"/>
-      <c r="K54" s="126"/>
-      <c r="L54" s="126"/>
-      <c r="M54" s="126"/>
-      <c r="N54" s="126"/>
-      <c r="O54" s="126"/>
-      <c r="P54" s="126"/>
-      <c r="Q54" s="126"/>
-      <c r="R54" s="126"/>
-      <c r="S54" s="126"/>
-      <c r="T54" s="126"/>
-      <c r="U54" s="126"/>
-      <c r="V54" s="126"/>
-      <c r="W54" s="126"/>
-      <c r="X54" s="126"/>
-      <c r="Y54" s="126"/>
-      <c r="Z54" s="126"/>
+        <f aca="false">COUNTIF(G54:BC54,"*last*")</f>
+        <v>1</v>
+      </c>
+      <c r="G54" s="128"/>
+      <c r="H54" s="128"/>
+      <c r="I54" s="128"/>
+      <c r="J54" s="128"/>
+      <c r="K54" s="128"/>
+      <c r="L54" s="128"/>
+      <c r="M54" s="128"/>
+      <c r="N54" s="125" t="s">
+        <v>697</v>
+      </c>
+      <c r="O54" s="128"/>
+      <c r="P54" s="128"/>
+      <c r="Q54" s="128"/>
+      <c r="R54" s="125" t="n">
+        <v>10</v>
+      </c>
+      <c r="S54" s="125" t="n">
+        <v>12</v>
+      </c>
+      <c r="T54" s="128"/>
+      <c r="U54" s="128"/>
+      <c r="V54" s="128"/>
+      <c r="W54" s="128"/>
+      <c r="X54" s="128"/>
+      <c r="Y54" s="128"/>
+      <c r="Z54" s="128"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="124" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="B55" s="125" t="n">
-        <f aca="false">COUNTIF(G49:BA49,"&lt;&gt;")</f>
-        <v>4</v>
+        <f aca="false">COUNTIF(G55:BA55,"&lt;&gt;")</f>
+        <v>2</v>
       </c>
       <c r="C55" s="125" t="n">
-        <f aca="false">COUNTIF(G49:BB49,"1")</f>
+        <f aca="false">COUNTIF(G55:BB55,"1")</f>
         <v>0</v>
       </c>
       <c r="D55" s="125" t="n">
-        <f aca="false">COUNTIF(G49:BC49,"2")</f>
+        <f aca="false">COUNTIF(G55:BC55,"2")</f>
+        <v>1</v>
+      </c>
+      <c r="E55" s="125" t="n">
+        <f aca="false">COUNTIF(G55:BD55,"3")</f>
         <v>0</v>
       </c>
-      <c r="E55" s="125" t="n">
-        <f aca="false">COUNTIF(G49:BD49,"3")</f>
+      <c r="F55" s="125" t="n">
+        <f aca="false">COUNTIF(G55:BC55,"*last*")</f>
         <v>0</v>
       </c>
-      <c r="F55" s="125" t="n">
-        <f aca="false">COUNTIF(G49:BC49,"*last*")</f>
-        <v>1</v>
-      </c>
-      <c r="G55" s="127"/>
+      <c r="G55" s="126"/>
       <c r="H55" s="125" t="n">
-        <v>4</v>
-      </c>
-      <c r="I55" s="126"/>
-      <c r="J55" s="126"/>
-      <c r="K55" s="126"/>
-      <c r="L55" s="126"/>
-      <c r="M55" s="127"/>
-      <c r="N55" s="127"/>
-      <c r="O55" s="126"/>
-      <c r="P55" s="126"/>
-      <c r="Q55" s="126"/>
-      <c r="R55" s="126"/>
-      <c r="S55" s="126"/>
-      <c r="T55" s="126"/>
-      <c r="U55" s="126"/>
-      <c r="V55" s="126"/>
-      <c r="W55" s="126"/>
-      <c r="X55" s="126"/>
-      <c r="Y55" s="126"/>
-      <c r="Z55" s="126"/>
+        <v>9</v>
+      </c>
+      <c r="I55" s="125" t="n">
+        <v>2</v>
+      </c>
+      <c r="J55" s="128"/>
+      <c r="K55" s="128"/>
+      <c r="L55" s="128"/>
+      <c r="M55" s="128"/>
+      <c r="N55" s="128"/>
+      <c r="O55" s="128"/>
+      <c r="P55" s="128"/>
+      <c r="Q55" s="128"/>
+      <c r="R55" s="128"/>
+      <c r="S55" s="128"/>
+      <c r="T55" s="128"/>
+      <c r="U55" s="128"/>
+      <c r="V55" s="128"/>
+      <c r="W55" s="128"/>
+      <c r="X55" s="128"/>
+      <c r="Y55" s="128"/>
+      <c r="Z55" s="128"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="124" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="B56" s="125" t="n">
-        <f aca="false">COUNTIF(G50:BA50,"&lt;&gt;")</f>
-        <v>6</v>
+        <f aca="false">COUNTIF(G56:BA56,"&lt;&gt;")</f>
+        <v>1</v>
       </c>
       <c r="C56" s="125" t="n">
-        <f aca="false">COUNTIF(G50:BB50,"1")</f>
-        <v>3</v>
+        <f aca="false">COUNTIF(G56:BB56,"1")</f>
+        <v>0</v>
       </c>
       <c r="D56" s="125" t="n">
-        <f aca="false">COUNTIF(G50:BC50,"2")</f>
-        <v>1</v>
+        <f aca="false">COUNTIF(G56:BC56,"2")</f>
+        <v>0</v>
       </c>
       <c r="E56" s="125" t="n">
-        <f aca="false">COUNTIF(G50:BD50,"3")</f>
+        <f aca="false">COUNTIF(G56:BD56,"3")</f>
         <v>0</v>
       </c>
       <c r="F56" s="125" t="n">
-        <f aca="false">COUNTIF(G50:BC50,"*last*")</f>
+        <f aca="false">COUNTIF(G56:BC56,"*last*")</f>
         <v>0</v>
       </c>
       <c r="G56" s="126"/>
-      <c r="H56" s="126"/>
-      <c r="I56" s="126"/>
-      <c r="J56" s="125" t="s">
-        <v>695</v>
-      </c>
-      <c r="K56" s="126"/>
-      <c r="L56" s="126"/>
-      <c r="M56" s="127"/>
-      <c r="N56" s="127"/>
-      <c r="O56" s="126"/>
-      <c r="P56" s="126"/>
-      <c r="Q56" s="126"/>
-      <c r="R56" s="126"/>
-      <c r="S56" s="126"/>
-      <c r="T56" s="126"/>
-      <c r="U56" s="126"/>
-      <c r="V56" s="126"/>
-      <c r="W56" s="126"/>
-      <c r="X56" s="126"/>
-      <c r="Y56" s="126"/>
-      <c r="Z56" s="126"/>
+      <c r="H56" s="125" t="n">
+        <v>4</v>
+      </c>
+      <c r="I56" s="128"/>
+      <c r="J56" s="128"/>
+      <c r="K56" s="128"/>
+      <c r="L56" s="128"/>
+      <c r="M56" s="126"/>
+      <c r="N56" s="126"/>
+      <c r="O56" s="128"/>
+      <c r="P56" s="128"/>
+      <c r="Q56" s="128"/>
+      <c r="R56" s="128"/>
+      <c r="S56" s="128"/>
+      <c r="T56" s="128"/>
+      <c r="U56" s="128"/>
+      <c r="V56" s="128"/>
+      <c r="W56" s="128"/>
+      <c r="X56" s="128"/>
+      <c r="Y56" s="128"/>
+      <c r="Z56" s="128"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="124" t="s">
-        <v>251</v>
+        <v>687</v>
       </c>
       <c r="B57" s="125" t="n">
-        <f aca="false">COUNTIF(G51:BA51,"&lt;&gt;")</f>
-        <v>3</v>
+        <f aca="false">COUNTIF(G57:BA57,"&lt;&gt;")</f>
+        <v>1</v>
       </c>
       <c r="C57" s="125" t="n">
-        <f aca="false">COUNTIF(G51:BB51,"1")</f>
+        <f aca="false">COUNTIF(G57:BB57,"1")</f>
         <v>0</v>
       </c>
       <c r="D57" s="125" t="n">
-        <f aca="false">COUNTIF(G51:BC51,"2")</f>
+        <f aca="false">COUNTIF(G57:BC57,"2")</f>
         <v>0</v>
       </c>
       <c r="E57" s="125" t="n">
-        <f aca="false">COUNTIF(G51:BD51,"3")</f>
+        <f aca="false">COUNTIF(G57:BD57,"3")</f>
         <v>0</v>
       </c>
       <c r="F57" s="125" t="n">
-        <f aca="false">COUNTIF(G51:BC51,"*last*")</f>
-        <v>0</v>
-      </c>
-      <c r="G57" s="126"/>
-      <c r="H57" s="126"/>
-      <c r="I57" s="126"/>
-      <c r="J57" s="126"/>
-      <c r="K57" s="126"/>
-      <c r="L57" s="126"/>
+        <f aca="false">COUNTIF(G57:BC57,"*last*")</f>
+        <v>1</v>
+      </c>
+      <c r="G57" s="128"/>
+      <c r="H57" s="128"/>
+      <c r="I57" s="128"/>
+      <c r="J57" s="125" t="s">
+        <v>696</v>
+      </c>
+      <c r="K57" s="128"/>
+      <c r="L57" s="128"/>
       <c r="M57" s="126"/>
       <c r="N57" s="126"/>
-      <c r="O57" s="126"/>
-      <c r="P57" s="126"/>
-      <c r="Q57" s="126"/>
-      <c r="R57" s="126"/>
-      <c r="S57" s="126"/>
-      <c r="T57" s="126"/>
-      <c r="U57" s="126"/>
-      <c r="V57" s="126"/>
-      <c r="W57" s="126"/>
-      <c r="X57" s="125" t="n">
-        <v>12</v>
-      </c>
-      <c r="Y57" s="125" t="n">
-        <v>9</v>
-      </c>
-      <c r="Z57" s="125" t="s">
-        <v>696</v>
-      </c>
+      <c r="O57" s="128"/>
+      <c r="P57" s="128"/>
+      <c r="Q57" s="128"/>
+      <c r="R57" s="128"/>
+      <c r="S57" s="128"/>
+      <c r="T57" s="128"/>
+      <c r="U57" s="128"/>
+      <c r="V57" s="128"/>
+      <c r="W57" s="128"/>
+      <c r="X57" s="128"/>
+      <c r="Y57" s="128"/>
+      <c r="Z57" s="128"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="124" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B58" s="125" t="n">
-        <f aca="false">COUNTIF(G52:BA52,"&lt;&gt;")</f>
-        <v>3</v>
+        <f aca="false">COUNTIF(G58:BA58,"&lt;&gt;")</f>
+        <v>0</v>
       </c>
       <c r="C58" s="125" t="n">
-        <f aca="false">COUNTIF(G52:BB52,"1")</f>
+        <f aca="false">COUNTIF(G58:BB58,"1")</f>
         <v>0</v>
       </c>
       <c r="D58" s="125" t="n">
-        <f aca="false">COUNTIF(G52:BC52,"2")</f>
+        <f aca="false">COUNTIF(G58:BC58,"2")</f>
         <v>0</v>
       </c>
       <c r="E58" s="125" t="n">
-        <f aca="false">COUNTIF(G52:BD52,"3")</f>
+        <f aca="false">COUNTIF(G58:BD58,"3")</f>
         <v>0</v>
       </c>
       <c r="F58" s="125" t="n">
-        <f aca="false">COUNTIF(G52:BC52,"*last*")</f>
-        <v>1</v>
-      </c>
-      <c r="G58" s="126"/>
-      <c r="H58" s="126"/>
-      <c r="I58" s="126"/>
-      <c r="J58" s="126"/>
-      <c r="K58" s="126"/>
-      <c r="L58" s="126"/>
-      <c r="M58" s="126"/>
-      <c r="N58" s="126"/>
-      <c r="O58" s="126"/>
-      <c r="P58" s="126"/>
-      <c r="Q58" s="126"/>
-      <c r="R58" s="126"/>
-      <c r="S58" s="126"/>
-      <c r="T58" s="126"/>
-      <c r="U58" s="126"/>
-      <c r="V58" s="126"/>
-      <c r="W58" s="126"/>
-      <c r="X58" s="126"/>
-      <c r="Y58" s="126"/>
-      <c r="Z58" s="126"/>
+        <f aca="false">COUNTIF(G58:BC58,"*last*")</f>
+        <v>0</v>
+      </c>
+      <c r="G58" s="128"/>
+      <c r="H58" s="128"/>
+      <c r="I58" s="128"/>
+      <c r="J58" s="128"/>
+      <c r="K58" s="128"/>
+      <c r="L58" s="128"/>
+      <c r="M58" s="128"/>
+      <c r="N58" s="128"/>
+      <c r="O58" s="128"/>
+      <c r="P58" s="128"/>
+      <c r="Q58" s="128"/>
+      <c r="R58" s="128"/>
+      <c r="S58" s="128"/>
+      <c r="T58" s="128"/>
+      <c r="U58" s="128"/>
+      <c r="V58" s="128"/>
+      <c r="W58" s="128"/>
+      <c r="X58" s="128"/>
+      <c r="Y58" s="128"/>
+      <c r="Z58" s="128"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="124" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="B59" s="125" t="n">
-        <f aca="false">COUNTIF(G53:BA53,"&lt;&gt;")</f>
-        <v>5</v>
+        <f aca="false">COUNTIF(G59:BA59,"&lt;&gt;")</f>
+        <v>0</v>
       </c>
       <c r="C59" s="125" t="n">
-        <f aca="false">COUNTIF(G53:BB53,"1")</f>
+        <f aca="false">COUNTIF(G59:BB59,"1")</f>
         <v>0</v>
       </c>
       <c r="D59" s="125" t="n">
-        <f aca="false">COUNTIF(G53:BC53,"2")</f>
+        <f aca="false">COUNTIF(G59:BC59,"2")</f>
         <v>0</v>
       </c>
       <c r="E59" s="125" t="n">
-        <f aca="false">COUNTIF(G53:BD53,"3")</f>
+        <f aca="false">COUNTIF(G59:BD59,"3")</f>
         <v>0</v>
       </c>
       <c r="F59" s="125" t="n">
-        <f aca="false">COUNTIF(G53:BC53,"*last*")</f>
-        <v>1</v>
-      </c>
-      <c r="G59" s="126"/>
-      <c r="H59" s="126"/>
-      <c r="I59" s="126"/>
-      <c r="J59" s="126"/>
-      <c r="K59" s="126"/>
-      <c r="L59" s="126"/>
-      <c r="M59" s="126"/>
-      <c r="N59" s="126"/>
-      <c r="O59" s="126"/>
-      <c r="P59" s="126"/>
-      <c r="Q59" s="126"/>
-      <c r="R59" s="126"/>
-      <c r="S59" s="126"/>
-      <c r="T59" s="126"/>
-      <c r="U59" s="126"/>
-      <c r="V59" s="126"/>
-      <c r="W59" s="126"/>
-      <c r="X59" s="126"/>
-      <c r="Y59" s="126"/>
-      <c r="Z59" s="126"/>
+        <f aca="false">COUNTIF(G59:BC59,"*last*")</f>
+        <v>0</v>
+      </c>
+      <c r="G59" s="128"/>
+      <c r="H59" s="128"/>
+      <c r="I59" s="128"/>
+      <c r="J59" s="128"/>
+      <c r="K59" s="128"/>
+      <c r="L59" s="128"/>
+      <c r="M59" s="128"/>
+      <c r="N59" s="128"/>
+      <c r="O59" s="128"/>
+      <c r="P59" s="128"/>
+      <c r="Q59" s="128"/>
+      <c r="R59" s="128"/>
+      <c r="S59" s="128"/>
+      <c r="T59" s="128"/>
+      <c r="U59" s="128"/>
+      <c r="V59" s="128"/>
+      <c r="W59" s="128"/>
+      <c r="X59" s="128"/>
+      <c r="Y59" s="128"/>
+      <c r="Z59" s="128"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -14118,7 +14116,7 @@
   </sheetPr>
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E33" activeCellId="0" sqref="E33"/>
     </sheetView>
   </sheetViews>
@@ -14680,7 +14678,7 @@
   </sheetPr>
   <dimension ref="A1:X105"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="T3" activeCellId="0" sqref="T3"/>
     </sheetView>
   </sheetViews>
@@ -16795,7 +16793,7 @@
   </sheetPr>
   <dimension ref="A1:W42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K31" activeCellId="0" sqref="K31"/>
     </sheetView>
   </sheetViews>
@@ -19067,7 +19065,7 @@
   </sheetPr>
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
@@ -19244,7 +19242,7 @@
   </sheetPr>
   <dimension ref="A1:A51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -19441,7 +19439,7 @@
   </sheetPr>
   <dimension ref="A1:AM17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="AD14" activeCellId="0" sqref="AD14"/>
     </sheetView>
   </sheetViews>
@@ -19463,7 +19461,7 @@
       </c>
       <c r="B1" s="0" t="n">
         <f aca="true">RAND()*100</f>
-        <v>2.55675854385492</v>
+        <v>76.0518163930504</v>
       </c>
       <c r="AA1" s="0" t="s">
         <v>356</v>
@@ -19511,7 +19509,7 @@
       </c>
       <c r="B2" s="0" t="n">
         <f aca="true">RAND()*100</f>
-        <v>35.3819856766353</v>
+        <v>53.1011021488601</v>
       </c>
       <c r="AB2" s="0" t="s">
         <v>175</v>
@@ -19556,7 +19554,7 @@
       </c>
       <c r="B3" s="0" t="n">
         <f aca="true">RAND()*100</f>
-        <v>64.3220610376793</v>
+        <v>3.29780781348404</v>
       </c>
       <c r="AC3" s="0" t="s">
         <v>355</v>
@@ -19850,7 +19848,7 @@
   </sheetPr>
   <dimension ref="A1:W42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -22885,7 +22883,7 @@
   </sheetPr>
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>

</xml_diff>